<commit_message>
fixes calculations and models because of a wrong value in literature
</commit_message>
<xml_diff>
--- a/proracun.xlsx
+++ b/proracun.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Faks\ek1\program 2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{532D31F1-7708-4BFD-ACCF-7975D924B790}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25ED8422-4E3C-4A43-A881-D138248AF645}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="5115" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="65">
   <si>
     <t>F</t>
   </si>
@@ -81,9 +81,6 @@
     <t>phi</t>
   </si>
   <si>
-    <t>rho</t>
-  </si>
-  <si>
     <t>samokočnost</t>
   </si>
   <si>
@@ -223,6 +220,15 @@
   </si>
   <si>
     <t>sigma_dopT</t>
+  </si>
+  <si>
+    <t>ispod matice</t>
+  </si>
+  <si>
+    <t>iznad matice</t>
+  </si>
+  <si>
+    <t>rho'</t>
   </si>
 </sst>
 </file>
@@ -231,7 +237,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="165" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="7">
     <font>
@@ -410,6 +416,9 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="2" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="3" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="5" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -422,9 +431,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="3" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="5" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Dobro" xfId="1" builtinId="26"/>
@@ -432,18 +438,11 @@
     <cellStyle name="Normalno" xfId="0" builtinId="0"/>
     <cellStyle name="Zarez" xfId="3" builtinId="3"/>
   </cellStyles>
-  <dxfs count="56">
+  <dxfs count="20">
     <dxf>
       <fill>
         <patternFill>
           <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF7575"/>
         </patternFill>
       </fill>
     </dxf>
@@ -464,252 +463,7 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF7171"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF7171"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF7171"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF7171"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF7171"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF6D6D"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF8181"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF8989"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
           <bgColor rgb="FFFF7575"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF7575"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF7171"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF7171"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF7171"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF7171"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF7171"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF6D6D"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF8181"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF8989"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1114,7 +868,7 @@
   <dimension ref="A2:W42"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="Y25" sqref="Y25"/>
+      <selection activeCell="Q19" sqref="Q19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -1125,7 +879,9 @@
     <col min="4" max="4" width="9.140625" style="3"/>
     <col min="5" max="5" width="12.42578125" style="3" customWidth="1"/>
     <col min="6" max="6" width="12.85546875" style="3" customWidth="1"/>
-    <col min="7" max="16" width="9.140625" style="3"/>
+    <col min="7" max="8" width="9.140625" style="3"/>
+    <col min="9" max="9" width="9.7109375" style="3" customWidth="1"/>
+    <col min="10" max="16" width="9.140625" style="3"/>
     <col min="17" max="17" width="10.7109375" style="3" customWidth="1"/>
     <col min="18" max="19" width="9.140625" style="3"/>
     <col min="20" max="20" width="12.5703125" style="3" customWidth="1"/>
@@ -1173,12 +929,16 @@
       <c r="F3" s="5"/>
       <c r="G3" s="7"/>
       <c r="H3" s="7"/>
-      <c r="I3" s="7"/>
-      <c r="J3" s="7"/>
+      <c r="I3" s="17" t="s">
+        <v>62</v>
+      </c>
+      <c r="J3" s="17"/>
       <c r="K3" s="7"/>
       <c r="L3" s="7"/>
-      <c r="M3" s="7"/>
-      <c r="N3" s="7"/>
+      <c r="M3" s="17" t="s">
+        <v>63</v>
+      </c>
+      <c r="N3" s="17"/>
       <c r="O3" s="7"/>
       <c r="P3" s="7"/>
       <c r="Q3" s="7"/>
@@ -1195,44 +955,44 @@
         <f>2*C3</f>
         <v>560</v>
       </c>
-      <c r="F4" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="G4" s="7" t="s">
+      <c r="F4" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="G4" s="11" t="s">
         <v>10</v>
       </c>
       <c r="H4" s="7"/>
       <c r="I4" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="J4" s="7">
         <f>ROUND(G7*G7*PI()/4,1)</f>
-        <v>637.9</v>
+        <v>397.6</v>
       </c>
       <c r="K4" s="7"/>
       <c r="L4" s="7"/>
       <c r="M4" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="N4" s="7">
         <f>ROUND(C2*G6/2*TAN((G11+G12)*PI()/180),0)</f>
-        <v>52188</v>
+        <v>56044</v>
       </c>
       <c r="O4" s="7"/>
       <c r="P4" s="7"/>
       <c r="Q4" s="7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="R4" s="7">
         <v>89</v>
       </c>
       <c r="S4" s="7"/>
       <c r="T4" s="7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="U4" s="6">
         <f>ROUND(4*C4/G7,2)</f>
-        <v>78.599999999999994</v>
+        <v>99.56</v>
       </c>
     </row>
     <row r="5" spans="2:21">
@@ -1242,28 +1002,28 @@
       <c r="C5" s="9">
         <v>250</v>
       </c>
-      <c r="F5" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="G5" s="7">
-        <v>24</v>
+      <c r="F5" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="G5" s="11">
+        <v>28</v>
       </c>
       <c r="H5" s="7"/>
       <c r="I5" s="7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J5" s="7">
         <f>ROUND(C2/J4,2)</f>
-        <v>29.79</v>
+        <v>47.79</v>
       </c>
       <c r="K5" s="7"/>
       <c r="L5" s="7"/>
       <c r="M5" s="7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="N5" s="7">
         <f>ROUND(POWER(G7,3)*PI()/16,1)</f>
-        <v>4545.3</v>
+        <v>2236.5</v>
       </c>
       <c r="O5" s="7"/>
       <c r="P5" s="7"/>
@@ -1274,11 +1034,11 @@
       <c r="U5" s="6"/>
     </row>
     <row r="6" spans="2:21">
-      <c r="F6" s="5" t="s">
+      <c r="F6" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="G6" s="7">
-        <v>21.5</v>
+      <c r="G6" s="11">
+        <v>25.5</v>
       </c>
       <c r="H6" s="7"/>
       <c r="I6" s="7"/>
@@ -1286,11 +1046,11 @@
       <c r="K6" s="7"/>
       <c r="L6" s="7"/>
       <c r="M6" s="7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="N6" s="7">
         <f>ROUND(N4/N5,2)</f>
-        <v>11.48</v>
+        <v>25.06</v>
       </c>
       <c r="O6" s="7"/>
       <c r="P6" s="7"/>
@@ -1307,11 +1067,11 @@
       <c r="C7" s="3">
         <v>210000</v>
       </c>
-      <c r="F7" s="5" t="s">
+      <c r="F7" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="G7" s="7">
-        <v>28.5</v>
+      <c r="G7" s="11">
+        <v>22.5</v>
       </c>
       <c r="H7" s="7"/>
       <c r="I7" s="7"/>
@@ -1323,19 +1083,19 @@
       <c r="O7" s="7"/>
       <c r="P7" s="7"/>
       <c r="Q7" s="7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="R7" s="7" t="b">
         <f>U4&gt;R4</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S7" s="7"/>
       <c r="T7" s="7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="U7" s="6" t="b">
         <f>U4&lt;R4</f>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="2:21">
@@ -1345,15 +1105,15 @@
       <c r="C8" s="3">
         <v>9</v>
       </c>
-      <c r="F8" s="5" t="s">
+      <c r="F8" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="G8" s="7">
+      <c r="G8" s="11">
         <v>5</v>
       </c>
       <c r="H8" s="7"/>
       <c r="I8" s="7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="J8" s="7">
         <v>300</v>
@@ -1361,7 +1121,7 @@
       <c r="K8" s="7"/>
       <c r="L8" s="7"/>
       <c r="M8" s="7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="N8" s="7">
         <v>190</v>
@@ -1381,16 +1141,16 @@
       <c r="C9" s="3">
         <v>0.1</v>
       </c>
-      <c r="F9" s="5" t="s">
+      <c r="F9" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="G9" s="7">
+      <c r="G9" s="11">
         <f>2*G8</f>
         <v>10</v>
       </c>
       <c r="H9" s="7"/>
       <c r="I9" s="7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="J9" s="7">
         <v>2.5</v>
@@ -1398,7 +1158,7 @@
       <c r="K9" s="7"/>
       <c r="L9" s="7"/>
       <c r="M9" s="7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="N9" s="7">
         <v>2.5</v>
@@ -1406,19 +1166,19 @@
       <c r="O9" s="7"/>
       <c r="P9" s="7"/>
       <c r="Q9" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="R9" s="7">
         <f>ROUND(PI()*PI()*C7/(U4*U4),1)</f>
-        <v>335.5</v>
+        <v>209.1</v>
       </c>
       <c r="S9" s="7"/>
       <c r="T9" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="U9" s="6">
         <f>ROUND(IF(R4=89,335-0.62*U4,310-1.14*U4),1)</f>
-        <v>286.3</v>
+        <v>273.3</v>
       </c>
     </row>
     <row r="10" spans="2:21">
@@ -1426,7 +1186,7 @@
       <c r="G10" s="7"/>
       <c r="H10" s="7"/>
       <c r="I10" s="7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="J10" s="7">
         <f>J8/J9</f>
@@ -1435,7 +1195,7 @@
       <c r="K10" s="7"/>
       <c r="L10" s="7"/>
       <c r="M10" s="7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="N10" s="7">
         <f>N8/N9</f>
@@ -1444,7 +1204,7 @@
       <c r="O10" s="7"/>
       <c r="P10" s="7"/>
       <c r="Q10" s="7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="R10" s="7">
         <f>ROUND(3+6/3*R4/250,2)</f>
@@ -1452,11 +1212,11 @@
       </c>
       <c r="S10" s="7"/>
       <c r="T10" s="7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="U10" s="6">
         <f>ROUND(2+4/2*U4*1/R4,2)</f>
-        <v>3.77</v>
+        <v>4.24</v>
       </c>
     </row>
     <row r="11" spans="2:21">
@@ -1465,7 +1225,7 @@
       </c>
       <c r="G11" s="7">
         <f>ROUND(ATAN(G9/(G6*PI()))*180/PI(),3)</f>
-        <v>8.4220000000000006</v>
+        <v>7.1150000000000002</v>
       </c>
       <c r="H11" s="7"/>
       <c r="I11" s="7"/>
@@ -1477,24 +1237,24 @@
       <c r="O11" s="7"/>
       <c r="P11" s="7"/>
       <c r="Q11" s="7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="R11" s="7">
         <f>ROUND(R9/J5,2)</f>
-        <v>11.26</v>
+        <v>4.38</v>
       </c>
       <c r="S11" s="7"/>
       <c r="T11" s="7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="U11" s="6">
         <f>ROUND(U9/J5,2)</f>
-        <v>9.61</v>
+        <v>5.72</v>
       </c>
     </row>
     <row r="12" spans="2:21">
       <c r="F12" s="5" t="s">
-        <v>15</v>
+        <v>64</v>
       </c>
       <c r="G12" s="7">
         <f>ROUND(ATAN(C9/COS(15*PI()/180))*180/PI(),3)</f>
@@ -1534,10 +1294,10 @@
       <c r="U13" s="6"/>
     </row>
     <row r="14" spans="2:21">
-      <c r="F14" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="G14" s="14"/>
+      <c r="F14" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="G14" s="17"/>
       <c r="H14" s="7"/>
       <c r="I14" s="7"/>
       <c r="J14" s="7"/>
@@ -1554,11 +1314,11 @@
       <c r="U14" s="6"/>
     </row>
     <row r="15" spans="2:21">
-      <c r="F15" s="15" t="b">
+      <c r="F15" s="18" t="b">
         <f>G11&lt;G12</f>
         <v>0</v>
       </c>
-      <c r="G15" s="16"/>
+      <c r="G15" s="19"/>
       <c r="H15" s="10"/>
       <c r="I15" s="10"/>
       <c r="J15" s="10"/>
@@ -1576,104 +1336,90 @@
     </row>
     <row r="17" spans="1:23">
       <c r="A17" s="1"/>
-      <c r="B17" s="4"/>
-      <c r="C17" s="4"/>
-      <c r="D17" s="4"/>
-      <c r="E17" s="4"/>
-      <c r="F17" s="4"/>
-      <c r="G17" s="2"/>
     </row>
     <row r="18" spans="1:23">
       <c r="A18" s="5"/>
-      <c r="B18" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="C18" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="D18" s="7"/>
-      <c r="E18" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="F18" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="G18" s="6"/>
+      <c r="B18" s="4"/>
+      <c r="C18" s="4"/>
+      <c r="D18" s="4"/>
+      <c r="E18" s="4"/>
+      <c r="F18" s="4"/>
+      <c r="G18" s="2"/>
       <c r="J18" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="K18" s="2">
         <f>G5</f>
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="M18" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="N18" s="2">
         <f>ROUND(N4/(C5/2),1)</f>
-        <v>417.5</v>
+        <v>448.4</v>
       </c>
       <c r="P18" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="Q18" s="4">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="R18" s="4"/>
       <c r="S18" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="T18" s="4">
         <f>ROUND(0.5*(Q19*Q19+2*Q18*Q19+Q18*Q20)/(Q18+Q19),2)</f>
-        <v>73.64</v>
+        <v>72.5</v>
       </c>
       <c r="U18" s="4"/>
       <c r="V18" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="W18" s="17">
+        <v>51</v>
+      </c>
+      <c r="W18" s="13">
         <f>C2*(C3-K19/2)</f>
-        <v>4750000</v>
+        <v>4655000</v>
       </c>
     </row>
     <row r="19" spans="1:23">
       <c r="A19" s="5"/>
       <c r="B19" s="11" t="s">
-        <v>37</v>
-      </c>
-      <c r="C19" s="11">
-        <v>36</v>
+        <v>9</v>
+      </c>
+      <c r="C19" s="11" t="s">
+        <v>10</v>
       </c>
       <c r="D19" s="7"/>
       <c r="E19" s="11" t="s">
-        <v>37</v>
-      </c>
-      <c r="F19" s="11">
-        <v>32</v>
+        <v>33</v>
+      </c>
+      <c r="F19" s="11" t="s">
+        <v>10</v>
       </c>
       <c r="G19" s="6"/>
       <c r="J19" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="K19" s="6">
         <f>K18*2.5</f>
-        <v>60</v>
+        <v>70</v>
       </c>
       <c r="M19" s="8" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="N19" s="9">
         <v>500</v>
       </c>
       <c r="P19" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="Q19" s="7">
         <v>100</v>
       </c>
       <c r="R19" s="7"/>
       <c r="S19" s="7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="T19" s="7">
         <f>Q19+Q20/2</f>
@@ -1681,40 +1427,40 @@
       </c>
       <c r="U19" s="7"/>
       <c r="V19" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="W19" s="18">
+        <v>52</v>
+      </c>
+      <c r="W19" s="14">
         <f>ROUND(Q18*POWER(Q20,3)/12+T21*T21*Q20*Q18+Q20*POWER(Q19,3)/12+T22*T22*Q20*Q19,0)</f>
-        <v>4546364</v>
+        <v>4406667</v>
       </c>
     </row>
     <row r="20" spans="1:23">
       <c r="A20" s="5"/>
       <c r="B20" s="11" t="s">
-        <v>11</v>
+        <v>36</v>
       </c>
       <c r="C20" s="11">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="D20" s="7"/>
       <c r="E20" s="11" t="s">
-        <v>11</v>
+        <v>36</v>
       </c>
       <c r="F20" s="11">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="G20" s="6"/>
       <c r="J20" s="5"/>
       <c r="K20" s="6"/>
       <c r="P20" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="Q20" s="7">
         <v>20</v>
       </c>
       <c r="R20" s="7"/>
       <c r="S20" s="7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="T20" s="7">
         <f>Q19/2</f>
@@ -1722,27 +1468,27 @@
       </c>
       <c r="U20" s="7"/>
       <c r="V20" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="W20" s="19">
+        <v>53</v>
+      </c>
+      <c r="W20" s="15">
         <f>W19/T18</f>
-        <v>61737.696903856602</v>
+        <v>60781.613793103446</v>
       </c>
     </row>
     <row r="21" spans="1:23">
       <c r="A21" s="5"/>
       <c r="B21" s="11" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="C21" s="11">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="D21" s="7"/>
       <c r="E21" s="11" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="F21" s="11">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="G21" s="6"/>
       <c r="J21" s="5" t="s">
@@ -1750,45 +1496,45 @@
       </c>
       <c r="K21" s="6">
         <f>G6</f>
-        <v>21.5</v>
+        <v>25.5</v>
       </c>
       <c r="P21" s="5"/>
       <c r="Q21" s="7"/>
       <c r="R21" s="7"/>
       <c r="S21" s="7" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="T21" s="7">
         <f>T19-T18</f>
-        <v>36.36</v>
+        <v>37.5</v>
       </c>
       <c r="U21" s="7"/>
       <c r="V21" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="W21" s="19">
+        <v>54</v>
+      </c>
+      <c r="W21" s="15">
         <f>W19/(Q19+Q20-T18)</f>
-        <v>98066.52286453839</v>
+        <v>92771.936842105264</v>
       </c>
     </row>
     <row r="22" spans="1:23">
       <c r="A22" s="5"/>
       <c r="B22" s="11" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="C22" s="11">
-        <v>6</v>
+        <v>29</v>
       </c>
       <c r="D22" s="7"/>
       <c r="E22" s="11" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="F22" s="11">
-        <v>6</v>
+        <v>25</v>
       </c>
       <c r="G22" s="6"/>
       <c r="J22" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="K22" s="6">
         <v>2.5</v>
@@ -1801,11 +1547,11 @@
       </c>
       <c r="R22" s="7"/>
       <c r="S22" s="7" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="T22" s="7">
         <f>T18-T20</f>
-        <v>23.64</v>
+        <v>22.5</v>
       </c>
       <c r="U22" s="7"/>
       <c r="V22" s="7"/>
@@ -1814,19 +1560,17 @@
     <row r="23" spans="1:23">
       <c r="A23" s="5"/>
       <c r="B23" s="11" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C23" s="11">
-        <f>2*C22</f>
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="D23" s="7"/>
       <c r="E23" s="11" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F23" s="11">
-        <f>2*F22</f>
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="G23" s="6"/>
       <c r="J23" s="5"/>
@@ -1842,14 +1586,24 @@
     </row>
     <row r="24" spans="1:23">
       <c r="A24" s="5"/>
-      <c r="B24" s="7"/>
-      <c r="C24" s="7"/>
+      <c r="B24" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="C24" s="11">
+        <f>2*C23</f>
+        <v>12</v>
+      </c>
       <c r="D24" s="7"/>
-      <c r="E24" s="7"/>
-      <c r="F24" s="7"/>
+      <c r="E24" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="F24" s="11">
+        <f>2*F23</f>
+        <v>12</v>
+      </c>
       <c r="G24" s="6"/>
       <c r="J24" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="K24" s="6">
         <v>10</v>
@@ -1865,38 +1619,30 @@
     </row>
     <row r="25" spans="1:23">
       <c r="A25" s="5"/>
-      <c r="B25" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="C25" s="11" t="s">
-        <v>10</v>
-      </c>
+      <c r="B25" s="7"/>
+      <c r="C25" s="7"/>
       <c r="D25" s="7"/>
-      <c r="E25" s="11" t="s">
-        <v>35</v>
-      </c>
-      <c r="F25" s="11" t="s">
-        <v>10</v>
-      </c>
+      <c r="E25" s="7"/>
+      <c r="F25" s="7"/>
       <c r="G25" s="6"/>
       <c r="J25" s="8" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="K25" s="9">
         <f>ROUND(C2*G8/(K21*PI()*K22*K19),2)</f>
-        <v>9.3800000000000008</v>
+        <v>6.78</v>
       </c>
       <c r="P25" s="5"/>
       <c r="Q25" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="R25" s="7">
         <f>-ROUND(W18/W20,2)</f>
-        <v>-76.94</v>
+        <v>-76.59</v>
       </c>
       <c r="S25" s="7"/>
       <c r="T25" s="7" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="U25" s="7">
         <v>58</v>
@@ -1907,30 +1653,30 @@
     <row r="26" spans="1:23">
       <c r="A26" s="5"/>
       <c r="B26" s="11" t="s">
-        <v>37</v>
-      </c>
-      <c r="C26" s="11">
-        <v>28</v>
+        <v>32</v>
+      </c>
+      <c r="C26" s="11" t="s">
+        <v>10</v>
       </c>
       <c r="D26" s="7"/>
-      <c r="E26" s="11" t="s">
-        <v>37</v>
-      </c>
-      <c r="F26" s="11">
-        <v>24</v>
+      <c r="E26" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="F26" s="12" t="s">
+        <v>10</v>
       </c>
       <c r="G26" s="6"/>
       <c r="P26" s="5"/>
       <c r="Q26" s="7" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="R26" s="7">
         <f>ROUND(W18/W21,2)</f>
-        <v>48.44</v>
+        <v>50.18</v>
       </c>
       <c r="S26" s="7"/>
       <c r="T26" s="7" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="U26" s="7">
         <v>72</v>
@@ -1941,26 +1687,26 @@
     <row r="27" spans="1:23">
       <c r="A27" s="5"/>
       <c r="B27" s="11" t="s">
-        <v>11</v>
+        <v>36</v>
       </c>
       <c r="C27" s="11">
-        <v>25.5</v>
+        <v>28</v>
       </c>
       <c r="D27" s="7"/>
-      <c r="E27" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="F27" s="11">
-        <v>21.5</v>
+      <c r="E27" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="F27" s="12">
+        <v>24</v>
       </c>
       <c r="G27" s="6"/>
       <c r="P27" s="5"/>
       <c r="Q27" s="7" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="R27" s="7">
         <f>ROUND(C2/(Q20*(Q18+Q19)),2)</f>
-        <v>5.76</v>
+        <v>5.94</v>
       </c>
       <c r="S27" s="7"/>
       <c r="T27" s="7"/>
@@ -1971,17 +1717,17 @@
     <row r="28" spans="1:23">
       <c r="A28" s="5"/>
       <c r="B28" s="11" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="C28" s="11">
-        <v>22.5</v>
+        <v>25.5</v>
       </c>
       <c r="D28" s="7"/>
-      <c r="E28" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="F28" s="11">
-        <v>28.5</v>
+      <c r="E28" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="F28" s="12">
+        <v>21.5</v>
       </c>
       <c r="G28" s="6"/>
       <c r="P28" s="5"/>
@@ -1989,11 +1735,11 @@
       <c r="R28" s="7"/>
       <c r="S28" s="7"/>
       <c r="T28" s="7" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="U28" s="7">
         <f>ABS(R25+R27)</f>
-        <v>71.179999999999993</v>
+        <v>70.650000000000006</v>
       </c>
       <c r="V28" s="7"/>
       <c r="W28" s="6"/>
@@ -2001,17 +1747,17 @@
     <row r="29" spans="1:23">
       <c r="A29" s="5"/>
       <c r="B29" s="11" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="C29" s="11">
-        <v>5</v>
+        <v>22.5</v>
       </c>
       <c r="D29" s="7"/>
-      <c r="E29" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="F29" s="11">
-        <v>5</v>
+      <c r="E29" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="F29" s="12">
+        <v>18.5</v>
       </c>
       <c r="G29" s="6"/>
       <c r="P29" s="8"/>
@@ -2019,11 +1765,11 @@
       <c r="R29" s="10"/>
       <c r="S29" s="10"/>
       <c r="T29" s="10" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="U29" s="10">
         <f>R26+R27</f>
-        <v>54.199999999999996</v>
+        <v>56.12</v>
       </c>
       <c r="V29" s="10"/>
       <c r="W29" s="9"/>
@@ -2031,39 +1777,43 @@
     <row r="30" spans="1:23">
       <c r="A30" s="5"/>
       <c r="B30" s="11" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C30" s="11">
-        <f>2*C29</f>
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="D30" s="7"/>
-      <c r="E30" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="F30" s="11">
-        <f>2*F29</f>
-        <v>10</v>
+      <c r="E30" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="F30" s="12">
+        <v>5</v>
       </c>
       <c r="G30" s="6"/>
     </row>
     <row r="31" spans="1:23">
       <c r="A31" s="5"/>
-      <c r="B31" s="7"/>
-      <c r="C31" s="7"/>
+      <c r="B31" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="C31" s="11">
+        <f>2*C30</f>
+        <v>10</v>
+      </c>
       <c r="D31" s="7"/>
-      <c r="E31" s="7"/>
-      <c r="F31" s="7"/>
+      <c r="E31" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="F31" s="12">
+        <f>2*F30</f>
+        <v>10</v>
+      </c>
       <c r="G31" s="6"/>
     </row>
     <row r="32" spans="1:23">
       <c r="A32" s="5"/>
-      <c r="B32" s="12" t="s">
-        <v>36</v>
-      </c>
-      <c r="C32" s="12" t="s">
-        <v>10</v>
-      </c>
+      <c r="B32" s="7"/>
+      <c r="C32" s="7"/>
       <c r="D32" s="7"/>
       <c r="E32" s="7"/>
       <c r="F32" s="7"/>
@@ -2072,10 +1822,10 @@
     <row r="33" spans="1:7">
       <c r="A33" s="5"/>
       <c r="B33" s="12" t="s">
-        <v>37</v>
-      </c>
-      <c r="C33" s="12">
-        <v>20</v>
+        <v>35</v>
+      </c>
+      <c r="C33" s="12" t="s">
+        <v>10</v>
       </c>
       <c r="D33" s="7"/>
       <c r="E33" s="7"/>
@@ -2085,10 +1835,10 @@
     <row r="34" spans="1:7">
       <c r="A34" s="5"/>
       <c r="B34" s="12" t="s">
-        <v>11</v>
+        <v>36</v>
       </c>
       <c r="C34" s="12">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="D34" s="7"/>
       <c r="E34" s="7"/>
@@ -2098,10 +1848,10 @@
     <row r="35" spans="1:7">
       <c r="A35" s="5"/>
       <c r="B35" s="12" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="C35" s="12">
-        <v>15.5</v>
+        <v>18</v>
       </c>
       <c r="D35" s="7"/>
       <c r="E35" s="7"/>
@@ -2111,10 +1861,10 @@
     <row r="36" spans="1:7">
       <c r="A36" s="5"/>
       <c r="B36" s="12" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="C36" s="12">
-        <v>4</v>
+        <v>15.5</v>
       </c>
       <c r="D36" s="7"/>
       <c r="E36" s="7"/>
@@ -2124,11 +1874,10 @@
     <row r="37" spans="1:7">
       <c r="A37" s="5"/>
       <c r="B37" s="12" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C37" s="12">
-        <f>2*C36</f>
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="D37" s="7"/>
       <c r="E37" s="7"/>
@@ -2137,12 +1886,25 @@
     </row>
     <row r="38" spans="1:7">
       <c r="A38" s="8"/>
-      <c r="B38" s="10"/>
-      <c r="C38" s="10"/>
-      <c r="D38" s="10"/>
-      <c r="E38" s="10"/>
-      <c r="F38" s="10"/>
-      <c r="G38" s="9"/>
+      <c r="B38" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="C38" s="12">
+        <f>2*C37</f>
+        <v>8</v>
+      </c>
+      <c r="D38" s="7"/>
+      <c r="E38" s="7"/>
+      <c r="F38" s="7"/>
+      <c r="G38" s="6"/>
+    </row>
+    <row r="39" spans="1:7">
+      <c r="B39" s="10"/>
+      <c r="C39" s="10"/>
+      <c r="D39" s="10"/>
+      <c r="E39" s="10"/>
+      <c r="F39" s="10"/>
+      <c r="G39" s="9"/>
     </row>
     <row r="40" spans="1:7">
       <c r="B40" s="7"/>
@@ -2160,87 +1922,89 @@
       <c r="D42" s="7"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="4">
     <mergeCell ref="F14:G14"/>
     <mergeCell ref="F15:G15"/>
+    <mergeCell ref="I3:J3"/>
+    <mergeCell ref="M3:N3"/>
   </mergeCells>
   <conditionalFormatting sqref="F15:G15">
-    <cfRule type="cellIs" dxfId="39" priority="21" operator="equal">
+    <cfRule type="cellIs" dxfId="19" priority="21" operator="equal">
       <formula>FALSE</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="38" priority="22" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="22" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J5">
-    <cfRule type="cellIs" dxfId="37" priority="19" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="17" priority="19" operator="greaterThan">
       <formula>$J$10</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="36" priority="20" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="16" priority="20" operator="lessThanOrEqual">
       <formula>$J$10</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N6">
-    <cfRule type="cellIs" dxfId="35" priority="17" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="15" priority="17" operator="greaterThan">
       <formula>$N$10</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="34" priority="18" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="14" priority="18" operator="lessThanOrEqual">
       <formula>$N$10</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R7">
-    <cfRule type="cellIs" dxfId="33" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="15" operator="equal">
       <formula>FALSE</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="32" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="16" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U7">
-    <cfRule type="cellIs" dxfId="31" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="13" operator="equal">
       <formula>FALSE</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="30" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="14" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U11">
-    <cfRule type="cellIs" dxfId="29" priority="9" operator="lessThan">
+    <cfRule type="cellIs" dxfId="9" priority="9" operator="lessThan">
       <formula>$U$10</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="28" priority="10" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="8" priority="10" operator="greaterThanOrEqual">
       <formula>$U$10</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R11">
-    <cfRule type="cellIs" dxfId="27" priority="7" operator="lessThan">
+    <cfRule type="cellIs" dxfId="7" priority="7" operator="lessThan">
       <formula>$R$10</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="26" priority="8" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="6" priority="8" operator="greaterThanOrEqual">
       <formula>$R$10</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K25">
-    <cfRule type="cellIs" dxfId="25" priority="5" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="5" priority="5" operator="greaterThan">
       <formula>$K$24</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="24" priority="6" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="4" priority="6" operator="lessThanOrEqual">
       <formula>$K$24</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U28">
-    <cfRule type="cellIs" dxfId="23" priority="4" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="3" priority="3" operator="greaterThan">
       <formula>$U$26</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="22" priority="3" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="2" priority="4" operator="lessThanOrEqual">
       <formula>$U$26</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U29">
-    <cfRule type="cellIs" dxfId="21" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="greaterThan">
       <formula>$U$25</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="20" priority="2" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="0" priority="2" operator="lessThanOrEqual">
       <formula>$U$25</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
modified calculations for required safety factor 1.5-3
</commit_message>
<xml_diff>
--- a/proracun.xlsx
+++ b/proracun.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Faks\ek1\program 2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25ED8422-4E3C-4A43-A881-D138248AF645}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE6B4FE0-1485-4B49-BFE3-81DA6766EB94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="5115" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="66">
   <si>
     <t>F</t>
   </si>
@@ -229,6 +229,9 @@
   </si>
   <si>
     <t>rho'</t>
+  </si>
+  <si>
+    <t>A</t>
   </si>
 </sst>
 </file>
@@ -868,7 +871,7 @@
   <dimension ref="A2:W42"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="Q19" sqref="Q19"/>
+      <selection activeCell="X8" sqref="X8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -1363,7 +1366,7 @@
         <v>43</v>
       </c>
       <c r="Q18" s="4">
-        <v>60</v>
+        <v>90</v>
       </c>
       <c r="R18" s="4"/>
       <c r="S18" s="4" t="s">
@@ -1371,7 +1374,7 @@
       </c>
       <c r="T18" s="4">
         <f>ROUND(0.5*(Q19*Q19+2*Q18*Q19+Q18*Q20)/(Q18+Q19),2)</f>
-        <v>72.5</v>
+        <v>63.41</v>
       </c>
       <c r="U18" s="4"/>
       <c r="V18" s="4" t="s">
@@ -1415,7 +1418,7 @@
         <v>44</v>
       </c>
       <c r="Q19" s="7">
-        <v>100</v>
+        <v>75</v>
       </c>
       <c r="R19" s="7"/>
       <c r="S19" s="7" t="s">
@@ -1423,7 +1426,7 @@
       </c>
       <c r="T19" s="7">
         <f>Q19+Q20/2</f>
-        <v>110</v>
+        <v>85</v>
       </c>
       <c r="U19" s="7"/>
       <c r="V19" s="7" t="s">
@@ -1431,7 +1434,7 @@
       </c>
       <c r="W19" s="14">
         <f>ROUND(Q18*POWER(Q20,3)/12+T21*T21*Q20*Q18+Q20*POWER(Q19,3)/12+T22*T22*Q20*Q19,0)</f>
-        <v>4406667</v>
+        <v>2609148</v>
       </c>
     </row>
     <row r="20" spans="1:23">
@@ -1464,7 +1467,7 @@
       </c>
       <c r="T20" s="7">
         <f>Q19/2</f>
-        <v>50</v>
+        <v>37.5</v>
       </c>
       <c r="U20" s="7"/>
       <c r="V20" s="7" t="s">
@@ -1472,7 +1475,7 @@
       </c>
       <c r="W20" s="15">
         <f>W19/T18</f>
-        <v>60781.613793103446</v>
+        <v>41147.26383851128</v>
       </c>
     </row>
     <row r="21" spans="1:23">
@@ -1498,15 +1501,20 @@
         <f>G6</f>
         <v>25.5</v>
       </c>
-      <c r="P21" s="5"/>
-      <c r="Q21" s="7"/>
+      <c r="P21" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="Q21" s="7">
+        <f>Q20*(Q18+Q19)</f>
+        <v>3300</v>
+      </c>
       <c r="R21" s="7"/>
       <c r="S21" s="7" t="s">
         <v>49</v>
       </c>
       <c r="T21" s="7">
         <f>T19-T18</f>
-        <v>37.5</v>
+        <v>21.590000000000003</v>
       </c>
       <c r="U21" s="7"/>
       <c r="V21" s="7" t="s">
@@ -1514,7 +1522,7 @@
       </c>
       <c r="W21" s="15">
         <f>W19/(Q19+Q20-T18)</f>
-        <v>92771.936842105264</v>
+        <v>82594.112060778716</v>
       </c>
     </row>
     <row r="22" spans="1:23">
@@ -1539,19 +1547,14 @@
       <c r="K22" s="6">
         <v>2.5</v>
       </c>
-      <c r="P22" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="Q22" s="7">
-        <v>2.5</v>
-      </c>
+      <c r="P22" s="5"/>
       <c r="R22" s="7"/>
       <c r="S22" s="7" t="s">
         <v>50</v>
       </c>
       <c r="T22" s="7">
         <f>T18-T20</f>
-        <v>22.5</v>
+        <v>25.909999999999997</v>
       </c>
       <c r="U22" s="7"/>
       <c r="V22" s="7"/>
@@ -1638,14 +1641,14 @@
       </c>
       <c r="R25" s="7">
         <f>-ROUND(W18/W20,2)</f>
-        <v>-76.59</v>
+        <v>-113.13</v>
       </c>
       <c r="S25" s="7"/>
       <c r="T25" s="7" t="s">
         <v>60</v>
       </c>
       <c r="U25" s="7">
-        <v>58</v>
+        <v>160</v>
       </c>
       <c r="V25" s="7"/>
       <c r="W25" s="6"/>
@@ -1672,14 +1675,14 @@
       </c>
       <c r="R26" s="7">
         <f>ROUND(W18/W21,2)</f>
-        <v>50.18</v>
+        <v>56.36</v>
       </c>
       <c r="S26" s="7"/>
       <c r="T26" s="7" t="s">
         <v>61</v>
       </c>
       <c r="U26" s="7">
-        <v>72</v>
+        <v>190</v>
       </c>
       <c r="V26" s="7"/>
       <c r="W26" s="6"/>
@@ -1705,8 +1708,8 @@
         <v>57</v>
       </c>
       <c r="R27" s="7">
-        <f>ROUND(C2/(Q20*(Q18+Q19)),2)</f>
-        <v>5.94</v>
+        <f>ROUND(C2/Q21,2)</f>
+        <v>5.76</v>
       </c>
       <c r="S27" s="7"/>
       <c r="T27" s="7"/>
@@ -1739,9 +1742,12 @@
       </c>
       <c r="U28" s="7">
         <f>ABS(R25+R27)</f>
-        <v>70.650000000000006</v>
-      </c>
-      <c r="V28" s="7"/>
+        <v>107.36999999999999</v>
+      </c>
+      <c r="V28" s="7">
+        <f>ROUND(U26/U28,2)</f>
+        <v>1.77</v>
+      </c>
       <c r="W28" s="6"/>
     </row>
     <row r="29" spans="1:23">
@@ -1769,9 +1775,12 @@
       </c>
       <c r="U29" s="10">
         <f>R26+R27</f>
-        <v>56.12</v>
-      </c>
-      <c r="V29" s="10"/>
+        <v>62.12</v>
+      </c>
+      <c r="V29" s="10">
+        <f>ROUND(U25/U29,2)</f>
+        <v>2.58</v>
+      </c>
       <c r="W29" s="9"/>
     </row>
     <row r="30" spans="1:23">

</xml_diff>

<commit_message>
fixed error in calculation of d3_potr
</commit_message>
<xml_diff>
--- a/proracun.xlsx
+++ b/proracun.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Faks\ek1\program 2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE6B4FE0-1485-4B49-BFE3-81DA6766EB94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D8D4BDA-EFE0-43A2-8E91-F560386998FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="5115" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -871,7 +871,7 @@
   <dimension ref="A2:W42"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="X8" sqref="X8"/>
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -904,8 +904,8 @@
         <v>8</v>
       </c>
       <c r="G2" s="4">
-        <f>ROUND(POWER((64*C2*C8*C4*C4)/(C7*PI()*PI()),0.25),2)</f>
-        <v>35.869999999999997</v>
+        <f>ROUND(POWER((64*C2*C8*C4*C4)/(C7*PI()*PI()*PI()),0.25),2)</f>
+        <v>26.94</v>
       </c>
       <c r="H2" s="4"/>
       <c r="I2" s="4"/>

</xml_diff>

<commit_message>
fixed sizes of threaded holes on parts with metric threads
</commit_message>
<xml_diff>
--- a/proracun.xlsx
+++ b/proracun.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Faks\ek1\program 2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D8D4BDA-EFE0-43A2-8E91-F560386998FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FA34FBE-0CF9-4C96-B45A-0659B871C009}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="5115" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -871,7 +871,7 @@
   <dimension ref="A2:W42"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+      <selection activeCell="W10" sqref="W10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -1210,15 +1210,15 @@
         <v>23</v>
       </c>
       <c r="R10" s="7">
-        <f>ROUND(3+6/3*R4/250,2)</f>
-        <v>3.71</v>
+        <f>ROUND(3+(U4-R4)*(6-3)/(250-R4),2)</f>
+        <v>3.2</v>
       </c>
       <c r="S10" s="7"/>
       <c r="T10" s="7" t="s">
         <v>23</v>
       </c>
       <c r="U10" s="6">
-        <f>ROUND(2+4/2*U4*1/R4,2)</f>
+        <f>ROUND(2+(U4-0)*(4-2)/(R4-0),2)</f>
         <v>4.24</v>
       </c>
     </row>

</xml_diff>

<commit_message>
fixed calculation, retouched drawings and models accordingly
</commit_message>
<xml_diff>
--- a/proracun.xlsx
+++ b/proracun.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Faks\ek1\program 2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FA34FBE-0CF9-4C96-B45A-0659B871C009}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1BC9E07-9448-42C2-A1B3-BB293B84AA2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="5115" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -870,8 +870,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:W42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="W10" sqref="W10"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="E42" sqref="E42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -958,6 +958,7 @@
         <f>2*C3</f>
         <v>560</v>
       </c>
+      <c r="E4" s="6"/>
       <c r="F4" s="11" t="s">
         <v>32</v>
       </c>
@@ -1005,6 +1006,7 @@
       <c r="C5" s="9">
         <v>250</v>
       </c>
+      <c r="E5" s="6"/>
       <c r="F5" s="11" t="s">
         <v>36</v>
       </c>
@@ -1037,6 +1039,7 @@
       <c r="U5" s="6"/>
     </row>
     <row r="6" spans="2:21">
+      <c r="E6" s="6"/>
       <c r="F6" s="11" t="s">
         <v>11</v>
       </c>
@@ -1070,6 +1073,7 @@
       <c r="C7" s="3">
         <v>210000</v>
       </c>
+      <c r="E7" s="6"/>
       <c r="F7" s="11" t="s">
         <v>7</v>
       </c>
@@ -1108,6 +1112,7 @@
       <c r="C8" s="3">
         <v>9</v>
       </c>
+      <c r="E8" s="6"/>
       <c r="F8" s="11" t="s">
         <v>13</v>
       </c>
@@ -1144,6 +1149,7 @@
       <c r="C9" s="3">
         <v>0.1</v>
       </c>
+      <c r="E9" s="6"/>
       <c r="F9" s="11" t="s">
         <v>12</v>
       </c>
@@ -1337,11 +1343,8 @@
       <c r="T15" s="10"/>
       <c r="U15" s="9"/>
     </row>
-    <row r="17" spans="1:23">
-      <c r="A17" s="1"/>
-    </row>
     <row r="18" spans="1:23">
-      <c r="A18" s="5"/>
+      <c r="A18" s="1"/>
       <c r="B18" s="4"/>
       <c r="C18" s="4"/>
       <c r="D18" s="4"/>
@@ -1374,7 +1377,7 @@
       </c>
       <c r="T18" s="4">
         <f>ROUND(0.5*(Q19*Q19+2*Q18*Q19+Q18*Q20)/(Q18+Q19),2)</f>
-        <v>63.41</v>
+        <v>58.91</v>
       </c>
       <c r="U18" s="4"/>
       <c r="V18" s="4" t="s">
@@ -1418,7 +1421,7 @@
         <v>44</v>
       </c>
       <c r="Q19" s="7">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="R19" s="7"/>
       <c r="S19" s="7" t="s">
@@ -1426,7 +1429,7 @@
       </c>
       <c r="T19" s="7">
         <f>Q19+Q20/2</f>
-        <v>85</v>
+        <v>77.5</v>
       </c>
       <c r="U19" s="7"/>
       <c r="V19" s="7" t="s">
@@ -1434,7 +1437,7 @@
       </c>
       <c r="W19" s="14">
         <f>ROUND(Q18*POWER(Q20,3)/12+T21*T21*Q20*Q18+Q20*POWER(Q19,3)/12+T22*T22*Q20*Q19,0)</f>
-        <v>2609148</v>
+        <v>1520879</v>
       </c>
     </row>
     <row r="20" spans="1:23">
@@ -1459,7 +1462,7 @@
         <v>45</v>
       </c>
       <c r="Q20" s="7">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="R20" s="7"/>
       <c r="S20" s="7" t="s">
@@ -1467,7 +1470,7 @@
       </c>
       <c r="T20" s="7">
         <f>Q19/2</f>
-        <v>37.5</v>
+        <v>35</v>
       </c>
       <c r="U20" s="7"/>
       <c r="V20" s="7" t="s">
@@ -1475,7 +1478,7 @@
       </c>
       <c r="W20" s="15">
         <f>W19/T18</f>
-        <v>41147.26383851128</v>
+        <v>25816.99202172806</v>
       </c>
     </row>
     <row r="21" spans="1:23">
@@ -1506,7 +1509,7 @@
       </c>
       <c r="Q21" s="7">
         <f>Q20*(Q18+Q19)</f>
-        <v>3300</v>
+        <v>2400</v>
       </c>
       <c r="R21" s="7"/>
       <c r="S21" s="7" t="s">
@@ -1514,7 +1517,7 @@
       </c>
       <c r="T21" s="7">
         <f>T19-T18</f>
-        <v>21.590000000000003</v>
+        <v>18.590000000000003</v>
       </c>
       <c r="U21" s="7"/>
       <c r="V21" s="7" t="s">
@@ -1522,7 +1525,7 @@
       </c>
       <c r="W21" s="15">
         <f>W19/(Q19+Q20-T18)</f>
-        <v>82594.112060778716</v>
+        <v>58293.560751245677</v>
       </c>
     </row>
     <row r="22" spans="1:23">
@@ -1554,7 +1557,7 @@
       </c>
       <c r="T22" s="7">
         <f>T18-T20</f>
-        <v>25.909999999999997</v>
+        <v>23.909999999999997</v>
       </c>
       <c r="U22" s="7"/>
       <c r="V22" s="7"/>
@@ -1641,7 +1644,7 @@
       </c>
       <c r="R25" s="7">
         <f>-ROUND(W18/W20,2)</f>
-        <v>-113.13</v>
+        <v>-180.31</v>
       </c>
       <c r="S25" s="7"/>
       <c r="T25" s="7" t="s">
@@ -1675,14 +1678,14 @@
       </c>
       <c r="R26" s="7">
         <f>ROUND(W18/W21,2)</f>
-        <v>56.36</v>
+        <v>79.849999999999994</v>
       </c>
       <c r="S26" s="7"/>
       <c r="T26" s="7" t="s">
         <v>61</v>
       </c>
       <c r="U26" s="7">
-        <v>190</v>
+        <v>500</v>
       </c>
       <c r="V26" s="7"/>
       <c r="W26" s="6"/>
@@ -1709,7 +1712,7 @@
       </c>
       <c r="R27" s="7">
         <f>ROUND(C2/Q21,2)</f>
-        <v>5.76</v>
+        <v>7.92</v>
       </c>
       <c r="S27" s="7"/>
       <c r="T27" s="7"/>
@@ -1742,11 +1745,11 @@
       </c>
       <c r="U28" s="7">
         <f>ABS(R25+R27)</f>
-        <v>107.36999999999999</v>
+        <v>172.39000000000001</v>
       </c>
       <c r="V28" s="7">
         <f>ROUND(U26/U28,2)</f>
-        <v>1.77</v>
+        <v>2.9</v>
       </c>
       <c r="W28" s="6"/>
     </row>
@@ -1775,11 +1778,11 @@
       </c>
       <c r="U29" s="10">
         <f>R26+R27</f>
-        <v>62.12</v>
+        <v>87.77</v>
       </c>
       <c r="V29" s="10">
         <f>ROUND(U25/U29,2)</f>
-        <v>2.58</v>
+        <v>1.82</v>
       </c>
       <c r="W29" s="9"/>
     </row>
@@ -1894,7 +1897,6 @@
       <c r="G37" s="6"/>
     </row>
     <row r="38" spans="1:7">
-      <c r="A38" s="8"/>
       <c r="B38" s="12" t="s">
         <v>12</v>
       </c>
@@ -1908,6 +1910,7 @@
       <c r="G38" s="6"/>
     </row>
     <row r="39" spans="1:7">
+      <c r="A39" s="8"/>
       <c r="B39" s="10"/>
       <c r="C39" s="10"/>
       <c r="D39" s="10"/>

</xml_diff>

<commit_message>
fixed number of decimals for some values and added calculation of H1
</commit_message>
<xml_diff>
--- a/proracun.xlsx
+++ b/proracun.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Faks\ek1\program 2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1BC9E07-9448-42C2-A1B3-BB293B84AA2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3300608E-D2DB-4F51-B849-6767C71FFCDC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="5115" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -405,7 +405,7 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
@@ -434,6 +434,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Dobro" xfId="1" builtinId="26"/>
@@ -870,8 +871,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:W42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="E42" sqref="E42"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="X15" sqref="X15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -1215,7 +1216,7 @@
       <c r="Q10" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="R10" s="7">
+      <c r="R10" s="20">
         <f>ROUND(3+(U4-R4)*(6-3)/(250-R4),2)</f>
         <v>3.2</v>
       </c>
@@ -1548,6 +1549,7 @@
         <v>38</v>
       </c>
       <c r="K22" s="6">
+        <f>G8/2</f>
         <v>2.5</v>
       </c>
       <c r="P22" s="5"/>
@@ -1747,7 +1749,7 @@
         <f>ABS(R25+R27)</f>
         <v>172.39000000000001</v>
       </c>
-      <c r="V28" s="7">
+      <c r="V28" s="20">
         <f>ROUND(U26/U28,2)</f>
         <v>2.9</v>
       </c>

</xml_diff>

<commit_message>
fixed allowed stress values and adjusted a, b, t accordingly
</commit_message>
<xml_diff>
--- a/proracun.xlsx
+++ b/proracun.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28129"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Faks\ek1\program 2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\David\Desktop\ek1\prog2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3300608E-D2DB-4F51-B849-6767C71FFCDC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11CA8BB3-2DFC-41B4-A09F-E262EEBBD709}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="5115" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="List1" sheetId="1" r:id="rId1"/>
@@ -242,7 +242,7 @@
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -405,7 +405,7 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
@@ -413,7 +413,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
@@ -422,10 +421,11 @@
     <xf numFmtId="164" fontId="3" fillId="0" borderId="3" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="5" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -434,7 +434,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Dobro" xfId="1" builtinId="26"/>
@@ -537,21 +536,21 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor rgb="FFFF6D6D"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor rgb="FFFF7171"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF6D6D"/>
         </patternFill>
       </fill>
     </dxf>
@@ -869,32 +868,32 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:W42"/>
+  <dimension ref="A2:W39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="X15" sqref="X15"/>
+    <sheetView tabSelected="1" topLeftCell="D9" workbookViewId="0">
+      <selection activeCell="N21" sqref="N21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="3"/>
-    <col min="2" max="2" width="12.5703125" style="3" customWidth="1"/>
-    <col min="3" max="3" width="10.42578125" style="3" customWidth="1"/>
-    <col min="4" max="4" width="9.140625" style="3"/>
-    <col min="5" max="5" width="12.42578125" style="3" customWidth="1"/>
-    <col min="6" max="6" width="12.85546875" style="3" customWidth="1"/>
-    <col min="7" max="8" width="9.140625" style="3"/>
-    <col min="9" max="9" width="9.7109375" style="3" customWidth="1"/>
-    <col min="10" max="16" width="9.140625" style="3"/>
-    <col min="17" max="17" width="10.7109375" style="3" customWidth="1"/>
-    <col min="18" max="19" width="9.140625" style="3"/>
-    <col min="20" max="20" width="12.5703125" style="3" customWidth="1"/>
-    <col min="21" max="22" width="9.140625" style="3"/>
-    <col min="23" max="23" width="15.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="24" max="16384" width="9.140625" style="3"/>
+    <col min="1" max="1" width="9.109375" style="3"/>
+    <col min="2" max="2" width="12.5546875" style="3" customWidth="1"/>
+    <col min="3" max="3" width="10.44140625" style="3" customWidth="1"/>
+    <col min="4" max="4" width="9.109375" style="3"/>
+    <col min="5" max="5" width="12.44140625" style="3" customWidth="1"/>
+    <col min="6" max="6" width="12.88671875" style="3" customWidth="1"/>
+    <col min="7" max="8" width="9.109375" style="3"/>
+    <col min="9" max="9" width="9.6640625" style="3" customWidth="1"/>
+    <col min="10" max="16" width="9.109375" style="3"/>
+    <col min="17" max="17" width="10.6640625" style="3" customWidth="1"/>
+    <col min="18" max="19" width="9.109375" style="3"/>
+    <col min="20" max="20" width="12.5546875" style="3" customWidth="1"/>
+    <col min="21" max="22" width="9.109375" style="3"/>
+    <col min="23" max="23" width="15.6640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="24" max="16384" width="9.109375" style="3"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:21">
+    <row r="2" spans="2:21" x14ac:dyDescent="0.3">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
@@ -923,7 +922,7 @@
       <c r="T2" s="4"/>
       <c r="U2" s="2"/>
     </row>
-    <row r="3" spans="2:21">
+    <row r="3" spans="2:21" x14ac:dyDescent="0.3">
       <c r="B3" s="5" t="s">
         <v>1</v>
       </c>
@@ -931,27 +930,17 @@
         <v>280</v>
       </c>
       <c r="F3" s="5"/>
-      <c r="G3" s="7"/>
-      <c r="H3" s="7"/>
       <c r="I3" s="17" t="s">
         <v>62</v>
       </c>
       <c r="J3" s="17"/>
-      <c r="K3" s="7"/>
-      <c r="L3" s="7"/>
       <c r="M3" s="17" t="s">
         <v>63</v>
       </c>
       <c r="N3" s="17"/>
-      <c r="O3" s="7"/>
-      <c r="P3" s="7"/>
-      <c r="Q3" s="7"/>
-      <c r="R3" s="7"/>
-      <c r="S3" s="7"/>
-      <c r="T3" s="7"/>
       <c r="U3" s="6"/>
     </row>
-    <row r="4" spans="2:21">
+    <row r="4" spans="2:21" x14ac:dyDescent="0.3">
       <c r="B4" s="5" t="s">
         <v>2</v>
       </c>
@@ -960,39 +949,33 @@
         <v>560</v>
       </c>
       <c r="E4" s="6"/>
-      <c r="F4" s="11" t="s">
+      <c r="F4" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="G4" s="11" t="s">
+      <c r="G4" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="H4" s="7"/>
-      <c r="I4" s="7" t="s">
+      <c r="I4" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="J4" s="7">
+      <c r="J4" s="3">
         <f>ROUND(G7*G7*PI()/4,1)</f>
         <v>397.6</v>
       </c>
-      <c r="K4" s="7"/>
-      <c r="L4" s="7"/>
-      <c r="M4" s="7" t="s">
+      <c r="M4" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="N4" s="7">
+      <c r="N4" s="3">
         <f>ROUND(C2*G6/2*TAN((G11+G12)*PI()/180),0)</f>
         <v>56044</v>
       </c>
-      <c r="O4" s="7"/>
-      <c r="P4" s="7"/>
-      <c r="Q4" s="7" t="s">
+      <c r="Q4" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="R4" s="7">
+      <c r="R4" s="3">
         <v>89</v>
       </c>
-      <c r="S4" s="7"/>
-      <c r="T4" s="7" t="s">
+      <c r="T4" s="3" t="s">
         <v>26</v>
       </c>
       <c r="U4" s="6">
@@ -1000,74 +983,54 @@
         <v>99.56</v>
       </c>
     </row>
-    <row r="5" spans="2:21">
-      <c r="B5" s="8" t="s">
+    <row r="5" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="B5" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="9">
+      <c r="C5" s="8">
         <v>250</v>
       </c>
       <c r="E5" s="6"/>
-      <c r="F5" s="11" t="s">
+      <c r="F5" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="G5" s="11">
+      <c r="G5" s="10">
         <v>28</v>
       </c>
-      <c r="H5" s="7"/>
-      <c r="I5" s="7" t="s">
+      <c r="I5" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="J5" s="7">
+      <c r="J5" s="3">
         <f>ROUND(C2/J4,2)</f>
         <v>47.79</v>
       </c>
-      <c r="K5" s="7"/>
-      <c r="L5" s="7"/>
-      <c r="M5" s="7" t="s">
+      <c r="M5" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="N5" s="7">
+      <c r="N5" s="3">
         <f>ROUND(POWER(G7,3)*PI()/16,1)</f>
         <v>2236.5</v>
       </c>
-      <c r="O5" s="7"/>
-      <c r="P5" s="7"/>
-      <c r="Q5" s="7"/>
-      <c r="R5" s="7"/>
-      <c r="S5" s="7"/>
-      <c r="T5" s="7"/>
       <c r="U5" s="6"/>
     </row>
-    <row r="6" spans="2:21">
+    <row r="6" spans="2:21" x14ac:dyDescent="0.3">
       <c r="E6" s="6"/>
-      <c r="F6" s="11" t="s">
+      <c r="F6" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="G6" s="11">
+      <c r="G6" s="10">
         <v>25.5</v>
       </c>
-      <c r="H6" s="7"/>
-      <c r="I6" s="7"/>
-      <c r="J6" s="7"/>
-      <c r="K6" s="7"/>
-      <c r="L6" s="7"/>
-      <c r="M6" s="7" t="s">
+      <c r="M6" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="N6" s="7">
+      <c r="N6" s="3">
         <f>ROUND(N4/N5,2)</f>
         <v>25.06</v>
       </c>
-      <c r="O6" s="7"/>
-      <c r="P6" s="7"/>
-      <c r="Q6" s="7"/>
-      <c r="R6" s="7"/>
-      <c r="S6" s="7"/>
-      <c r="T6" s="7"/>
       <c r="U6" s="6"/>
     </row>
-    <row r="7" spans="2:21">
+    <row r="7" spans="2:21" x14ac:dyDescent="0.3">
       <c r="B7" s="3" t="s">
         <v>5</v>
       </c>
@@ -1075,30 +1038,20 @@
         <v>210000</v>
       </c>
       <c r="E7" s="6"/>
-      <c r="F7" s="11" t="s">
+      <c r="F7" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="G7" s="11">
+      <c r="G7" s="10">
         <v>22.5</v>
       </c>
-      <c r="H7" s="7"/>
-      <c r="I7" s="7"/>
-      <c r="J7" s="7"/>
-      <c r="K7" s="7"/>
-      <c r="L7" s="7"/>
-      <c r="M7" s="7"/>
-      <c r="N7" s="7"/>
-      <c r="O7" s="7"/>
-      <c r="P7" s="7"/>
-      <c r="Q7" s="7" t="s">
+      <c r="Q7" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="R7" s="7" t="b">
+      <c r="R7" s="3" t="b">
         <f>U4&gt;R4</f>
         <v>1</v>
       </c>
-      <c r="S7" s="7"/>
-      <c r="T7" s="7" t="s">
+      <c r="T7" s="3" t="s">
         <v>29</v>
       </c>
       <c r="U7" s="6" t="b">
@@ -1106,7 +1059,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="2:21">
+    <row r="8" spans="2:21" x14ac:dyDescent="0.3">
       <c r="B8" s="3" t="s">
         <v>4</v>
       </c>
@@ -1114,36 +1067,27 @@
         <v>9</v>
       </c>
       <c r="E8" s="6"/>
-      <c r="F8" s="11" t="s">
+      <c r="F8" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="G8" s="11">
+      <c r="G8" s="10">
         <v>5</v>
       </c>
-      <c r="H8" s="7"/>
-      <c r="I8" s="7" t="s">
+      <c r="I8" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="J8" s="7">
+      <c r="J8" s="3">
         <v>300</v>
       </c>
-      <c r="K8" s="7"/>
-      <c r="L8" s="7"/>
-      <c r="M8" s="7" t="s">
+      <c r="M8" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="N8" s="7">
+      <c r="N8" s="3">
         <v>190</v>
       </c>
-      <c r="O8" s="7"/>
-      <c r="P8" s="7"/>
-      <c r="Q8" s="7"/>
-      <c r="R8" s="7"/>
-      <c r="S8" s="7"/>
-      <c r="T8" s="7"/>
       <c r="U8" s="6"/>
     </row>
-    <row r="9" spans="2:21">
+    <row r="9" spans="2:21" x14ac:dyDescent="0.3">
       <c r="B9" s="3" t="s">
         <v>6</v>
       </c>
@@ -1151,39 +1095,33 @@
         <v>0.1</v>
       </c>
       <c r="E9" s="6"/>
-      <c r="F9" s="11" t="s">
+      <c r="F9" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="G9" s="11">
+      <c r="G9" s="10">
         <f>2*G8</f>
         <v>10</v>
       </c>
-      <c r="H9" s="7"/>
-      <c r="I9" s="7" t="s">
+      <c r="I9" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="J9" s="7">
+      <c r="J9" s="3">
         <v>2.5</v>
       </c>
-      <c r="K9" s="7"/>
-      <c r="L9" s="7"/>
-      <c r="M9" s="7" t="s">
+      <c r="M9" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="N9" s="7">
+      <c r="N9" s="3">
         <v>2.5</v>
       </c>
-      <c r="O9" s="7"/>
-      <c r="P9" s="7"/>
-      <c r="Q9" s="7" t="s">
+      <c r="Q9" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="R9" s="7">
+      <c r="R9" s="3">
         <f>ROUND(PI()*PI()*C7/(U4*U4),1)</f>
         <v>209.1</v>
       </c>
-      <c r="S9" s="7"/>
-      <c r="T9" s="7" t="s">
+      <c r="T9" s="3" t="s">
         <v>30</v>
       </c>
       <c r="U9" s="6">
@@ -1191,37 +1129,30 @@
         <v>273.3</v>
       </c>
     </row>
-    <row r="10" spans="2:21">
+    <row r="10" spans="2:21" x14ac:dyDescent="0.3">
       <c r="F10" s="5"/>
-      <c r="G10" s="7"/>
-      <c r="H10" s="7"/>
-      <c r="I10" s="7" t="s">
+      <c r="I10" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="J10" s="7">
+      <c r="J10" s="3">
         <f>J8/J9</f>
         <v>120</v>
       </c>
-      <c r="K10" s="7"/>
-      <c r="L10" s="7"/>
-      <c r="M10" s="7" t="s">
+      <c r="M10" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="N10" s="7">
+      <c r="N10" s="3">
         <f>N8/N9</f>
         <v>76</v>
       </c>
-      <c r="O10" s="7"/>
-      <c r="P10" s="7"/>
-      <c r="Q10" s="7" t="s">
+      <c r="Q10" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="R10" s="20">
+      <c r="R10" s="15">
         <f>ROUND(3+(U4-R4)*(6-3)/(250-R4),2)</f>
         <v>3.2</v>
       </c>
-      <c r="S10" s="7"/>
-      <c r="T10" s="7" t="s">
+      <c r="T10" s="3" t="s">
         <v>23</v>
       </c>
       <c r="U10" s="6">
@@ -1229,32 +1160,22 @@
         <v>4.24</v>
       </c>
     </row>
-    <row r="11" spans="2:21">
+    <row r="11" spans="2:21" x14ac:dyDescent="0.3">
       <c r="F11" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="G11" s="7">
+      <c r="G11" s="3">
         <f>ROUND(ATAN(G9/(G6*PI()))*180/PI(),3)</f>
         <v>7.1150000000000002</v>
       </c>
-      <c r="H11" s="7"/>
-      <c r="I11" s="7"/>
-      <c r="J11" s="7"/>
-      <c r="K11" s="7"/>
-      <c r="L11" s="7"/>
-      <c r="M11" s="7"/>
-      <c r="N11" s="7"/>
-      <c r="O11" s="7"/>
-      <c r="P11" s="7"/>
-      <c r="Q11" s="7" t="s">
+      <c r="Q11" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="R11" s="7">
+      <c r="R11" s="3">
         <f>ROUND(R9/J5,2)</f>
         <v>4.38</v>
       </c>
-      <c r="S11" s="7"/>
-      <c r="T11" s="7" t="s">
+      <c r="T11" s="3" t="s">
         <v>31</v>
       </c>
       <c r="U11" s="6">
@@ -1262,89 +1183,49 @@
         <v>5.72</v>
       </c>
     </row>
-    <row r="12" spans="2:21">
+    <row r="12" spans="2:21" x14ac:dyDescent="0.3">
       <c r="F12" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="G12" s="7">
+      <c r="G12" s="3">
         <f>ROUND(ATAN(C9/COS(15*PI()/180))*180/PI(),3)</f>
         <v>5.9109999999999996</v>
       </c>
-      <c r="H12" s="7"/>
-      <c r="I12" s="7"/>
-      <c r="J12" s="7"/>
-      <c r="K12" s="7"/>
-      <c r="L12" s="7"/>
-      <c r="M12" s="7"/>
-      <c r="N12" s="7"/>
-      <c r="O12" s="7"/>
-      <c r="P12" s="7"/>
-      <c r="Q12" s="7"/>
-      <c r="R12" s="7"/>
-      <c r="S12" s="7"/>
-      <c r="T12" s="7"/>
       <c r="U12" s="6"/>
     </row>
-    <row r="13" spans="2:21">
+    <row r="13" spans="2:21" x14ac:dyDescent="0.3">
       <c r="F13" s="5"/>
-      <c r="G13" s="7"/>
-      <c r="H13" s="7"/>
-      <c r="I13" s="7"/>
-      <c r="J13" s="7"/>
-      <c r="K13" s="7"/>
-      <c r="L13" s="7"/>
-      <c r="M13" s="7"/>
-      <c r="N13" s="7"/>
-      <c r="O13" s="7"/>
-      <c r="P13" s="7"/>
-      <c r="Q13" s="7"/>
-      <c r="R13" s="7"/>
-      <c r="S13" s="7"/>
-      <c r="T13" s="7"/>
       <c r="U13" s="6"/>
     </row>
-    <row r="14" spans="2:21">
+    <row r="14" spans="2:21" x14ac:dyDescent="0.3">
       <c r="F14" s="16" t="s">
         <v>15</v>
       </c>
       <c r="G14" s="17"/>
-      <c r="H14" s="7"/>
-      <c r="I14" s="7"/>
-      <c r="J14" s="7"/>
-      <c r="K14" s="7"/>
-      <c r="L14" s="7"/>
-      <c r="M14" s="7"/>
-      <c r="N14" s="7"/>
-      <c r="O14" s="7"/>
-      <c r="P14" s="7"/>
-      <c r="Q14" s="7"/>
-      <c r="R14" s="7"/>
-      <c r="S14" s="7"/>
-      <c r="T14" s="7"/>
       <c r="U14" s="6"/>
     </row>
-    <row r="15" spans="2:21">
+    <row r="15" spans="2:21" x14ac:dyDescent="0.3">
       <c r="F15" s="18" t="b">
         <f>G11&lt;G12</f>
         <v>0</v>
       </c>
       <c r="G15" s="19"/>
-      <c r="H15" s="10"/>
-      <c r="I15" s="10"/>
-      <c r="J15" s="10"/>
-      <c r="K15" s="10"/>
-      <c r="L15" s="10"/>
-      <c r="M15" s="10"/>
-      <c r="N15" s="10"/>
-      <c r="O15" s="10"/>
-      <c r="P15" s="10"/>
-      <c r="Q15" s="10"/>
-      <c r="R15" s="10"/>
-      <c r="S15" s="10"/>
-      <c r="T15" s="10"/>
-      <c r="U15" s="9"/>
-    </row>
-    <row r="18" spans="1:23">
+      <c r="H15" s="9"/>
+      <c r="I15" s="9"/>
+      <c r="J15" s="9"/>
+      <c r="K15" s="9"/>
+      <c r="L15" s="9"/>
+      <c r="M15" s="9"/>
+      <c r="N15" s="9"/>
+      <c r="O15" s="9"/>
+      <c r="P15" s="9"/>
+      <c r="Q15" s="9"/>
+      <c r="R15" s="9"/>
+      <c r="S15" s="9"/>
+      <c r="T15" s="9"/>
+      <c r="U15" s="8"/>
+    </row>
+    <row r="18" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A18" s="1"/>
       <c r="B18" s="4"/>
       <c r="C18" s="4"/>
@@ -1370,7 +1251,7 @@
         <v>43</v>
       </c>
       <c r="Q18" s="4">
-        <v>90</v>
+        <v>110</v>
       </c>
       <c r="R18" s="4"/>
       <c r="S18" s="4" t="s">
@@ -1378,30 +1259,29 @@
       </c>
       <c r="T18" s="4">
         <f>ROUND(0.5*(Q19*Q19+2*Q18*Q19+Q18*Q20)/(Q18+Q19),2)</f>
-        <v>58.91</v>
+        <v>76.63</v>
       </c>
       <c r="U18" s="4"/>
       <c r="V18" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="W18" s="13">
+      <c r="W18" s="12">
         <f>C2*(C3-K19/2)</f>
         <v>4655000</v>
       </c>
     </row>
-    <row r="19" spans="1:23">
+    <row r="19" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A19" s="5"/>
-      <c r="B19" s="11" t="s">
+      <c r="B19" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="C19" s="11" t="s">
+      <c r="C19" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="D19" s="7"/>
-      <c r="E19" s="11" t="s">
+      <c r="E19" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="F19" s="11" t="s">
+      <c r="F19" s="10" t="s">
         <v>10</v>
       </c>
       <c r="G19" s="6"/>
@@ -1412,48 +1292,45 @@
         <f>K18*2.5</f>
         <v>70</v>
       </c>
-      <c r="M19" s="8" t="s">
+      <c r="M19" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="N19" s="9">
+      <c r="N19" s="8">
         <v>500</v>
       </c>
       <c r="P19" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="Q19" s="7">
-        <v>70</v>
-      </c>
-      <c r="R19" s="7"/>
-      <c r="S19" s="7" t="s">
+      <c r="Q19" s="3">
+        <v>90</v>
+      </c>
+      <c r="S19" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="T19" s="7">
+      <c r="T19" s="3">
         <f>Q19+Q20/2</f>
-        <v>77.5</v>
-      </c>
-      <c r="U19" s="7"/>
-      <c r="V19" s="7" t="s">
+        <v>102.5</v>
+      </c>
+      <c r="V19" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="W19" s="14">
+      <c r="W19" s="13">
         <f>ROUND(Q18*POWER(Q20,3)/12+T21*T21*Q20*Q18+Q20*POWER(Q19,3)/12+T22*T22*Q20*Q19,0)</f>
-        <v>1520879</v>
-      </c>
-    </row>
-    <row r="20" spans="1:23">
+        <v>5753464</v>
+      </c>
+    </row>
+    <row r="20" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A20" s="5"/>
-      <c r="B20" s="11" t="s">
+      <c r="B20" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="C20" s="11">
+      <c r="C20" s="10">
         <v>36</v>
       </c>
-      <c r="D20" s="7"/>
-      <c r="E20" s="11" t="s">
+      <c r="E20" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="F20" s="11">
+      <c r="F20" s="10">
         <v>32</v>
       </c>
       <c r="G20" s="6"/>
@@ -1462,39 +1339,36 @@
       <c r="P20" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="Q20" s="7">
-        <v>15</v>
-      </c>
-      <c r="R20" s="7"/>
-      <c r="S20" s="7" t="s">
+      <c r="Q20" s="3">
+        <v>25</v>
+      </c>
+      <c r="S20" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="T20" s="7">
+      <c r="T20" s="3">
         <f>Q19/2</f>
-        <v>35</v>
-      </c>
-      <c r="U20" s="7"/>
-      <c r="V20" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="V20" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="W20" s="15">
+      <c r="W20" s="14">
         <f>W19/T18</f>
-        <v>25816.99202172806</v>
-      </c>
-    </row>
-    <row r="21" spans="1:23">
+        <v>75081.090956544445</v>
+      </c>
+    </row>
+    <row r="21" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A21" s="5"/>
-      <c r="B21" s="11" t="s">
+      <c r="B21" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="C21" s="11">
+      <c r="C21" s="10">
         <v>33</v>
       </c>
-      <c r="D21" s="7"/>
-      <c r="E21" s="11" t="s">
+      <c r="E21" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="F21" s="11">
+      <c r="F21" s="10">
         <v>29</v>
       </c>
       <c r="G21" s="6"/>
@@ -1508,40 +1382,37 @@
       <c r="P21" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="Q21" s="7">
+      <c r="Q21" s="3">
         <f>Q20*(Q18+Q19)</f>
-        <v>2400</v>
-      </c>
-      <c r="R21" s="7"/>
-      <c r="S21" s="7" t="s">
+        <v>5000</v>
+      </c>
+      <c r="S21" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="T21" s="7">
+      <c r="T21" s="3">
         <f>T19-T18</f>
-        <v>18.590000000000003</v>
-      </c>
-      <c r="U21" s="7"/>
-      <c r="V21" s="7" t="s">
+        <v>25.870000000000005</v>
+      </c>
+      <c r="V21" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="W21" s="15">
+      <c r="W21" s="14">
         <f>W19/(Q19+Q20-T18)</f>
-        <v>58293.560751245677</v>
-      </c>
-    </row>
-    <row r="22" spans="1:23">
+        <v>149946.93771175397</v>
+      </c>
+    </row>
+    <row r="22" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A22" s="5"/>
-      <c r="B22" s="11" t="s">
+      <c r="B22" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="C22" s="11">
+      <c r="C22" s="10">
         <v>29</v>
       </c>
-      <c r="D22" s="7"/>
-      <c r="E22" s="11" t="s">
+      <c r="E22" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="F22" s="11">
+      <c r="F22" s="10">
         <v>25</v>
       </c>
       <c r="G22" s="6"/>
@@ -1553,59 +1424,48 @@
         <v>2.5</v>
       </c>
       <c r="P22" s="5"/>
-      <c r="R22" s="7"/>
-      <c r="S22" s="7" t="s">
+      <c r="S22" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="T22" s="7">
+      <c r="T22" s="3">
         <f>T18-T20</f>
-        <v>23.909999999999997</v>
-      </c>
-      <c r="U22" s="7"/>
-      <c r="V22" s="7"/>
+        <v>31.629999999999995</v>
+      </c>
       <c r="W22" s="6"/>
     </row>
-    <row r="23" spans="1:23">
+    <row r="23" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A23" s="5"/>
-      <c r="B23" s="11" t="s">
+      <c r="B23" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="C23" s="11">
+      <c r="C23" s="10">
         <v>6</v>
       </c>
-      <c r="D23" s="7"/>
-      <c r="E23" s="11" t="s">
+      <c r="E23" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="F23" s="11">
+      <c r="F23" s="10">
         <v>6</v>
       </c>
       <c r="G23" s="6"/>
       <c r="J23" s="5"/>
       <c r="K23" s="6"/>
       <c r="P23" s="5"/>
-      <c r="Q23" s="7"/>
-      <c r="R23" s="7"/>
-      <c r="S23" s="7"/>
-      <c r="T23" s="7"/>
-      <c r="U23" s="7"/>
-      <c r="V23" s="7"/>
       <c r="W23" s="6"/>
     </row>
-    <row r="24" spans="1:23">
+    <row r="24" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A24" s="5"/>
-      <c r="B24" s="11" t="s">
+      <c r="B24" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="C24" s="11">
+      <c r="C24" s="10">
         <f>2*C23</f>
         <v>12</v>
       </c>
-      <c r="D24" s="7"/>
-      <c r="E24" s="11" t="s">
+      <c r="E24" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="F24" s="11">
+      <c r="F24" s="10">
         <f>2*F23</f>
         <v>12</v>
       </c>
@@ -1617,323 +1477,257 @@
         <v>10</v>
       </c>
       <c r="P24" s="5"/>
-      <c r="Q24" s="7"/>
-      <c r="R24" s="7"/>
-      <c r="S24" s="7"/>
-      <c r="T24" s="7"/>
-      <c r="U24" s="7"/>
-      <c r="V24" s="7"/>
       <c r="W24" s="6"/>
     </row>
-    <row r="25" spans="1:23">
+    <row r="25" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A25" s="5"/>
-      <c r="B25" s="7"/>
-      <c r="C25" s="7"/>
-      <c r="D25" s="7"/>
-      <c r="E25" s="7"/>
-      <c r="F25" s="7"/>
       <c r="G25" s="6"/>
-      <c r="J25" s="8" t="s">
+      <c r="J25" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="K25" s="9">
+      <c r="K25" s="8">
         <f>ROUND(C2*G8/(K21*PI()*K22*K19),2)</f>
         <v>6.78</v>
       </c>
       <c r="P25" s="5"/>
-      <c r="Q25" s="7" t="s">
+      <c r="Q25" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="R25" s="7">
+      <c r="R25" s="3">
         <f>-ROUND(W18/W20,2)</f>
-        <v>-180.31</v>
-      </c>
-      <c r="S25" s="7"/>
-      <c r="T25" s="7" t="s">
+        <v>-62</v>
+      </c>
+      <c r="T25" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="U25" s="7">
-        <v>160</v>
-      </c>
-      <c r="V25" s="7"/>
+      <c r="U25" s="3">
+        <v>60</v>
+      </c>
       <c r="W25" s="6"/>
     </row>
-    <row r="26" spans="1:23">
+    <row r="26" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A26" s="5"/>
-      <c r="B26" s="11" t="s">
+      <c r="B26" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="C26" s="11" t="s">
+      <c r="C26" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="D26" s="7"/>
-      <c r="E26" s="12" t="s">
+      <c r="E26" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="F26" s="12" t="s">
+      <c r="F26" s="11" t="s">
         <v>10</v>
       </c>
       <c r="G26" s="6"/>
       <c r="P26" s="5"/>
-      <c r="Q26" s="7" t="s">
+      <c r="Q26" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="R26" s="7">
+      <c r="R26" s="3">
         <f>ROUND(W18/W21,2)</f>
-        <v>79.849999999999994</v>
-      </c>
-      <c r="S26" s="7"/>
-      <c r="T26" s="7" t="s">
+        <v>31.04</v>
+      </c>
+      <c r="T26" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="U26" s="7">
-        <v>500</v>
-      </c>
-      <c r="V26" s="7"/>
+      <c r="U26" s="3">
+        <v>160</v>
+      </c>
       <c r="W26" s="6"/>
     </row>
-    <row r="27" spans="1:23">
+    <row r="27" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A27" s="5"/>
-      <c r="B27" s="11" t="s">
+      <c r="B27" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="C27" s="11">
+      <c r="C27" s="10">
         <v>28</v>
       </c>
-      <c r="D27" s="7"/>
-      <c r="E27" s="12" t="s">
+      <c r="E27" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="F27" s="12">
+      <c r="F27" s="11">
         <v>24</v>
       </c>
       <c r="G27" s="6"/>
       <c r="P27" s="5"/>
-      <c r="Q27" s="7" t="s">
+      <c r="Q27" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="R27" s="7">
+      <c r="R27" s="3">
         <f>ROUND(C2/Q21,2)</f>
-        <v>7.92</v>
-      </c>
-      <c r="S27" s="7"/>
-      <c r="T27" s="7"/>
-      <c r="U27" s="7"/>
-      <c r="V27" s="7"/>
+        <v>3.8</v>
+      </c>
       <c r="W27" s="6"/>
     </row>
-    <row r="28" spans="1:23">
+    <row r="28" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A28" s="5"/>
-      <c r="B28" s="11" t="s">
+      <c r="B28" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="C28" s="11">
+      <c r="C28" s="10">
         <v>25.5</v>
       </c>
-      <c r="D28" s="7"/>
-      <c r="E28" s="12" t="s">
+      <c r="E28" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="F28" s="12">
+      <c r="F28" s="11">
         <v>21.5</v>
       </c>
       <c r="G28" s="6"/>
       <c r="P28" s="5"/>
-      <c r="Q28" s="7"/>
-      <c r="R28" s="7"/>
-      <c r="S28" s="7"/>
-      <c r="T28" s="7" t="s">
+      <c r="T28" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="U28" s="7">
+      <c r="U28" s="3">
         <f>ABS(R25+R27)</f>
-        <v>172.39000000000001</v>
-      </c>
-      <c r="V28" s="20">
+        <v>58.2</v>
+      </c>
+      <c r="V28" s="15">
         <f>ROUND(U26/U28,2)</f>
-        <v>2.9</v>
+        <v>2.75</v>
       </c>
       <c r="W28" s="6"/>
     </row>
-    <row r="29" spans="1:23">
+    <row r="29" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A29" s="5"/>
-      <c r="B29" s="11" t="s">
+      <c r="B29" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="C29" s="11">
+      <c r="C29" s="10">
         <v>22.5</v>
       </c>
-      <c r="D29" s="7"/>
-      <c r="E29" s="12" t="s">
+      <c r="E29" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="F29" s="12">
+      <c r="F29" s="11">
         <v>18.5</v>
       </c>
       <c r="G29" s="6"/>
-      <c r="P29" s="8"/>
-      <c r="Q29" s="10"/>
-      <c r="R29" s="10"/>
-      <c r="S29" s="10"/>
-      <c r="T29" s="10" t="s">
+      <c r="P29" s="7"/>
+      <c r="Q29" s="9"/>
+      <c r="R29" s="9"/>
+      <c r="S29" s="9"/>
+      <c r="T29" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="U29" s="10">
+      <c r="U29" s="9">
         <f>R26+R27</f>
-        <v>87.77</v>
-      </c>
-      <c r="V29" s="10">
+        <v>34.839999999999996</v>
+      </c>
+      <c r="V29" s="9">
         <f>ROUND(U25/U29,2)</f>
-        <v>1.82</v>
-      </c>
-      <c r="W29" s="9"/>
-    </row>
-    <row r="30" spans="1:23">
+        <v>1.72</v>
+      </c>
+      <c r="W29" s="8"/>
+    </row>
+    <row r="30" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A30" s="5"/>
-      <c r="B30" s="11" t="s">
+      <c r="B30" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="C30" s="11">
+      <c r="C30" s="10">
         <v>5</v>
       </c>
-      <c r="D30" s="7"/>
-      <c r="E30" s="12" t="s">
+      <c r="E30" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="F30" s="12">
+      <c r="F30" s="11">
         <v>5</v>
       </c>
       <c r="G30" s="6"/>
     </row>
-    <row r="31" spans="1:23">
+    <row r="31" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A31" s="5"/>
-      <c r="B31" s="11" t="s">
+      <c r="B31" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="C31" s="11">
+      <c r="C31" s="10">
         <f>2*C30</f>
         <v>10</v>
       </c>
-      <c r="D31" s="7"/>
-      <c r="E31" s="12" t="s">
+      <c r="E31" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="F31" s="12">
+      <c r="F31" s="11">
         <f>2*F30</f>
         <v>10</v>
       </c>
       <c r="G31" s="6"/>
     </row>
-    <row r="32" spans="1:23">
+    <row r="32" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A32" s="5"/>
-      <c r="B32" s="7"/>
-      <c r="C32" s="7"/>
-      <c r="D32" s="7"/>
-      <c r="E32" s="7"/>
-      <c r="F32" s="7"/>
       <c r="G32" s="6"/>
     </row>
-    <row r="33" spans="1:7">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A33" s="5"/>
-      <c r="B33" s="12" t="s">
+      <c r="B33" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="C33" s="12" t="s">
+      <c r="C33" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="D33" s="7"/>
-      <c r="E33" s="7"/>
-      <c r="F33" s="7"/>
       <c r="G33" s="6"/>
     </row>
-    <row r="34" spans="1:7">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A34" s="5"/>
-      <c r="B34" s="12" t="s">
+      <c r="B34" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="C34" s="12">
+      <c r="C34" s="11">
         <v>20</v>
       </c>
-      <c r="D34" s="7"/>
-      <c r="E34" s="7"/>
-      <c r="F34" s="7"/>
       <c r="G34" s="6"/>
     </row>
-    <row r="35" spans="1:7">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A35" s="5"/>
-      <c r="B35" s="12" t="s">
+      <c r="B35" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="C35" s="12">
+      <c r="C35" s="11">
         <v>18</v>
       </c>
-      <c r="D35" s="7"/>
-      <c r="E35" s="7"/>
-      <c r="F35" s="7"/>
       <c r="G35" s="6"/>
     </row>
-    <row r="36" spans="1:7">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A36" s="5"/>
-      <c r="B36" s="12" t="s">
+      <c r="B36" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="C36" s="12">
+      <c r="C36" s="11">
         <v>15.5</v>
       </c>
-      <c r="D36" s="7"/>
-      <c r="E36" s="7"/>
-      <c r="F36" s="7"/>
       <c r="G36" s="6"/>
     </row>
-    <row r="37" spans="1:7">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A37" s="5"/>
-      <c r="B37" s="12" t="s">
+      <c r="B37" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="C37" s="12">
+      <c r="C37" s="11">
         <v>4</v>
       </c>
-      <c r="D37" s="7"/>
-      <c r="E37" s="7"/>
-      <c r="F37" s="7"/>
       <c r="G37" s="6"/>
     </row>
-    <row r="38" spans="1:7">
-      <c r="B38" s="12" t="s">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B38" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="C38" s="12">
+      <c r="C38" s="11">
         <f>2*C37</f>
         <v>8</v>
       </c>
-      <c r="D38" s="7"/>
-      <c r="E38" s="7"/>
-      <c r="F38" s="7"/>
       <c r="G38" s="6"/>
     </row>
-    <row r="39" spans="1:7">
-      <c r="A39" s="8"/>
-      <c r="B39" s="10"/>
-      <c r="C39" s="10"/>
-      <c r="D39" s="10"/>
-      <c r="E39" s="10"/>
-      <c r="F39" s="10"/>
-      <c r="G39" s="9"/>
-    </row>
-    <row r="40" spans="1:7">
-      <c r="B40" s="7"/>
-      <c r="C40" s="7"/>
-      <c r="D40" s="7"/>
-    </row>
-    <row r="41" spans="1:7">
-      <c r="B41" s="7"/>
-      <c r="C41" s="7"/>
-      <c r="D41" s="7"/>
-    </row>
-    <row r="42" spans="1:7">
-      <c r="B42" s="7"/>
-      <c r="C42" s="7"/>
-      <c r="D42" s="7"/>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A39" s="7"/>
+      <c r="B39" s="9"/>
+      <c r="C39" s="9"/>
+      <c r="D39" s="9"/>
+      <c r="E39" s="9"/>
+      <c r="F39" s="9"/>
+      <c r="G39" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -1958,52 +1752,52 @@
       <formula>$J$10</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="K25">
+    <cfRule type="cellIs" dxfId="15" priority="5" operator="greaterThan">
+      <formula>$K$24</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="14" priority="6" operator="lessThanOrEqual">
+      <formula>$K$24</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="N6">
-    <cfRule type="cellIs" dxfId="15" priority="17" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="13" priority="17" operator="greaterThan">
       <formula>$N$10</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="14" priority="18" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="12" priority="18" operator="lessThanOrEqual">
       <formula>$N$10</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R7">
-    <cfRule type="cellIs" dxfId="13" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="15" operator="equal">
       <formula>FALSE</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="16" operator="equal">
       <formula>TRUE</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="R11">
+    <cfRule type="cellIs" dxfId="9" priority="7" operator="lessThan">
+      <formula>$R$10</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="8" priority="8" operator="greaterThanOrEqual">
+      <formula>$R$10</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U7">
-    <cfRule type="cellIs" dxfId="11" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="13" operator="equal">
       <formula>FALSE</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="14" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U11">
-    <cfRule type="cellIs" dxfId="9" priority="9" operator="lessThan">
+    <cfRule type="cellIs" dxfId="5" priority="9" operator="lessThan">
       <formula>$U$10</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="10" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="4" priority="10" operator="greaterThanOrEqual">
       <formula>$U$10</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="R11">
-    <cfRule type="cellIs" dxfId="7" priority="7" operator="lessThan">
-      <formula>$R$10</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="8" operator="greaterThanOrEqual">
-      <formula>$R$10</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K25">
-    <cfRule type="cellIs" dxfId="5" priority="5" operator="greaterThan">
-      <formula>$K$24</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="6" operator="lessThanOrEqual">
-      <formula>$K$24</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U28">

</xml_diff>

<commit_message>
Revert "fixed allowed stress values and adjusted a, b, t accordingly"
This reverts commit 788d713a750bf01a4f75b0579023316f215465bc.
</commit_message>
<xml_diff>
--- a/proracun.xlsx
+++ b/proracun.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24701"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\David\Desktop\ek1\prog2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Faks\ek1\program 2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11CA8BB3-2DFC-41B4-A09F-E262EEBBD709}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3300608E-D2DB-4F51-B849-6767C71FFCDC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="5115" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="List1" sheetId="1" r:id="rId1"/>
@@ -242,7 +242,7 @@
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -405,7 +405,7 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
@@ -413,6 +413,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
@@ -421,11 +422,10 @@
     <xf numFmtId="164" fontId="3" fillId="0" borderId="3" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="5" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -434,6 +434,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Dobro" xfId="1" builtinId="26"/>
@@ -536,7 +537,7 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFF6D6D"/>
+          <bgColor rgb="FFFF7171"/>
         </patternFill>
       </fill>
     </dxf>
@@ -550,7 +551,7 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFF7171"/>
+          <bgColor rgb="FFFF6D6D"/>
         </patternFill>
       </fill>
     </dxf>
@@ -868,32 +869,32 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:W39"/>
+  <dimension ref="A2:W42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D9" workbookViewId="0">
-      <selection activeCell="N21" sqref="N21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="X15" sqref="X15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="9.109375" style="3"/>
-    <col min="2" max="2" width="12.5546875" style="3" customWidth="1"/>
-    <col min="3" max="3" width="10.44140625" style="3" customWidth="1"/>
-    <col min="4" max="4" width="9.109375" style="3"/>
-    <col min="5" max="5" width="12.44140625" style="3" customWidth="1"/>
-    <col min="6" max="6" width="12.88671875" style="3" customWidth="1"/>
-    <col min="7" max="8" width="9.109375" style="3"/>
-    <col min="9" max="9" width="9.6640625" style="3" customWidth="1"/>
-    <col min="10" max="16" width="9.109375" style="3"/>
-    <col min="17" max="17" width="10.6640625" style="3" customWidth="1"/>
-    <col min="18" max="19" width="9.109375" style="3"/>
-    <col min="20" max="20" width="12.5546875" style="3" customWidth="1"/>
-    <col min="21" max="22" width="9.109375" style="3"/>
-    <col min="23" max="23" width="15.6640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="24" max="16384" width="9.109375" style="3"/>
+    <col min="1" max="1" width="9.140625" style="3"/>
+    <col min="2" max="2" width="12.5703125" style="3" customWidth="1"/>
+    <col min="3" max="3" width="10.42578125" style="3" customWidth="1"/>
+    <col min="4" max="4" width="9.140625" style="3"/>
+    <col min="5" max="5" width="12.42578125" style="3" customWidth="1"/>
+    <col min="6" max="6" width="12.85546875" style="3" customWidth="1"/>
+    <col min="7" max="8" width="9.140625" style="3"/>
+    <col min="9" max="9" width="9.7109375" style="3" customWidth="1"/>
+    <col min="10" max="16" width="9.140625" style="3"/>
+    <col min="17" max="17" width="10.7109375" style="3" customWidth="1"/>
+    <col min="18" max="19" width="9.140625" style="3"/>
+    <col min="20" max="20" width="12.5703125" style="3" customWidth="1"/>
+    <col min="21" max="22" width="9.140625" style="3"/>
+    <col min="23" max="23" width="15.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="24" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:21" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:21">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
@@ -922,7 +923,7 @@
       <c r="T2" s="4"/>
       <c r="U2" s="2"/>
     </row>
-    <row r="3" spans="2:21" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:21">
       <c r="B3" s="5" t="s">
         <v>1</v>
       </c>
@@ -930,17 +931,27 @@
         <v>280</v>
       </c>
       <c r="F3" s="5"/>
+      <c r="G3" s="7"/>
+      <c r="H3" s="7"/>
       <c r="I3" s="17" t="s">
         <v>62</v>
       </c>
       <c r="J3" s="17"/>
+      <c r="K3" s="7"/>
+      <c r="L3" s="7"/>
       <c r="M3" s="17" t="s">
         <v>63</v>
       </c>
       <c r="N3" s="17"/>
+      <c r="O3" s="7"/>
+      <c r="P3" s="7"/>
+      <c r="Q3" s="7"/>
+      <c r="R3" s="7"/>
+      <c r="S3" s="7"/>
+      <c r="T3" s="7"/>
       <c r="U3" s="6"/>
     </row>
-    <row r="4" spans="2:21" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:21">
       <c r="B4" s="5" t="s">
         <v>2</v>
       </c>
@@ -949,33 +960,39 @@
         <v>560</v>
       </c>
       <c r="E4" s="6"/>
-      <c r="F4" s="10" t="s">
+      <c r="F4" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="G4" s="10" t="s">
+      <c r="G4" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="I4" s="3" t="s">
+      <c r="H4" s="7"/>
+      <c r="I4" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="J4" s="3">
+      <c r="J4" s="7">
         <f>ROUND(G7*G7*PI()/4,1)</f>
         <v>397.6</v>
       </c>
-      <c r="M4" s="3" t="s">
+      <c r="K4" s="7"/>
+      <c r="L4" s="7"/>
+      <c r="M4" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="N4" s="3">
+      <c r="N4" s="7">
         <f>ROUND(C2*G6/2*TAN((G11+G12)*PI()/180),0)</f>
         <v>56044</v>
       </c>
-      <c r="Q4" s="3" t="s">
+      <c r="O4" s="7"/>
+      <c r="P4" s="7"/>
+      <c r="Q4" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="R4" s="3">
+      <c r="R4" s="7">
         <v>89</v>
       </c>
-      <c r="T4" s="3" t="s">
+      <c r="S4" s="7"/>
+      <c r="T4" s="7" t="s">
         <v>26</v>
       </c>
       <c r="U4" s="6">
@@ -983,54 +1000,74 @@
         <v>99.56</v>
       </c>
     </row>
-    <row r="5" spans="2:21" x14ac:dyDescent="0.3">
-      <c r="B5" s="7" t="s">
+    <row r="5" spans="2:21">
+      <c r="B5" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="8">
+      <c r="C5" s="9">
         <v>250</v>
       </c>
       <c r="E5" s="6"/>
-      <c r="F5" s="10" t="s">
+      <c r="F5" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="G5" s="10">
+      <c r="G5" s="11">
         <v>28</v>
       </c>
-      <c r="I5" s="3" t="s">
+      <c r="H5" s="7"/>
+      <c r="I5" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="J5" s="3">
+      <c r="J5" s="7">
         <f>ROUND(C2/J4,2)</f>
         <v>47.79</v>
       </c>
-      <c r="M5" s="3" t="s">
+      <c r="K5" s="7"/>
+      <c r="L5" s="7"/>
+      <c r="M5" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="N5" s="3">
+      <c r="N5" s="7">
         <f>ROUND(POWER(G7,3)*PI()/16,1)</f>
         <v>2236.5</v>
       </c>
+      <c r="O5" s="7"/>
+      <c r="P5" s="7"/>
+      <c r="Q5" s="7"/>
+      <c r="R5" s="7"/>
+      <c r="S5" s="7"/>
+      <c r="T5" s="7"/>
       <c r="U5" s="6"/>
     </row>
-    <row r="6" spans="2:21" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:21">
       <c r="E6" s="6"/>
-      <c r="F6" s="10" t="s">
+      <c r="F6" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="G6" s="10">
+      <c r="G6" s="11">
         <v>25.5</v>
       </c>
-      <c r="M6" s="3" t="s">
+      <c r="H6" s="7"/>
+      <c r="I6" s="7"/>
+      <c r="J6" s="7"/>
+      <c r="K6" s="7"/>
+      <c r="L6" s="7"/>
+      <c r="M6" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="N6" s="3">
+      <c r="N6" s="7">
         <f>ROUND(N4/N5,2)</f>
         <v>25.06</v>
       </c>
+      <c r="O6" s="7"/>
+      <c r="P6" s="7"/>
+      <c r="Q6" s="7"/>
+      <c r="R6" s="7"/>
+      <c r="S6" s="7"/>
+      <c r="T6" s="7"/>
       <c r="U6" s="6"/>
     </row>
-    <row r="7" spans="2:21" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:21">
       <c r="B7" s="3" t="s">
         <v>5</v>
       </c>
@@ -1038,20 +1075,30 @@
         <v>210000</v>
       </c>
       <c r="E7" s="6"/>
-      <c r="F7" s="10" t="s">
+      <c r="F7" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="G7" s="10">
+      <c r="G7" s="11">
         <v>22.5</v>
       </c>
-      <c r="Q7" s="3" t="s">
+      <c r="H7" s="7"/>
+      <c r="I7" s="7"/>
+      <c r="J7" s="7"/>
+      <c r="K7" s="7"/>
+      <c r="L7" s="7"/>
+      <c r="M7" s="7"/>
+      <c r="N7" s="7"/>
+      <c r="O7" s="7"/>
+      <c r="P7" s="7"/>
+      <c r="Q7" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="R7" s="3" t="b">
+      <c r="R7" s="7" t="b">
         <f>U4&gt;R4</f>
         <v>1</v>
       </c>
-      <c r="T7" s="3" t="s">
+      <c r="S7" s="7"/>
+      <c r="T7" s="7" t="s">
         <v>29</v>
       </c>
       <c r="U7" s="6" t="b">
@@ -1059,7 +1106,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="2:21" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:21">
       <c r="B8" s="3" t="s">
         <v>4</v>
       </c>
@@ -1067,27 +1114,36 @@
         <v>9</v>
       </c>
       <c r="E8" s="6"/>
-      <c r="F8" s="10" t="s">
+      <c r="F8" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="G8" s="10">
+      <c r="G8" s="11">
         <v>5</v>
       </c>
-      <c r="I8" s="3" t="s">
+      <c r="H8" s="7"/>
+      <c r="I8" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="J8" s="3">
+      <c r="J8" s="7">
         <v>300</v>
       </c>
-      <c r="M8" s="3" t="s">
+      <c r="K8" s="7"/>
+      <c r="L8" s="7"/>
+      <c r="M8" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="N8" s="3">
+      <c r="N8" s="7">
         <v>190</v>
       </c>
+      <c r="O8" s="7"/>
+      <c r="P8" s="7"/>
+      <c r="Q8" s="7"/>
+      <c r="R8" s="7"/>
+      <c r="S8" s="7"/>
+      <c r="T8" s="7"/>
       <c r="U8" s="6"/>
     </row>
-    <row r="9" spans="2:21" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:21">
       <c r="B9" s="3" t="s">
         <v>6</v>
       </c>
@@ -1095,33 +1151,39 @@
         <v>0.1</v>
       </c>
       <c r="E9" s="6"/>
-      <c r="F9" s="10" t="s">
+      <c r="F9" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="G9" s="10">
+      <c r="G9" s="11">
         <f>2*G8</f>
         <v>10</v>
       </c>
-      <c r="I9" s="3" t="s">
+      <c r="H9" s="7"/>
+      <c r="I9" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="J9" s="3">
+      <c r="J9" s="7">
         <v>2.5</v>
       </c>
-      <c r="M9" s="3" t="s">
+      <c r="K9" s="7"/>
+      <c r="L9" s="7"/>
+      <c r="M9" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="N9" s="3">
+      <c r="N9" s="7">
         <v>2.5</v>
       </c>
-      <c r="Q9" s="3" t="s">
+      <c r="O9" s="7"/>
+      <c r="P9" s="7"/>
+      <c r="Q9" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="R9" s="3">
+      <c r="R9" s="7">
         <f>ROUND(PI()*PI()*C7/(U4*U4),1)</f>
         <v>209.1</v>
       </c>
-      <c r="T9" s="3" t="s">
+      <c r="S9" s="7"/>
+      <c r="T9" s="7" t="s">
         <v>30</v>
       </c>
       <c r="U9" s="6">
@@ -1129,30 +1191,37 @@
         <v>273.3</v>
       </c>
     </row>
-    <row r="10" spans="2:21" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:21">
       <c r="F10" s="5"/>
-      <c r="I10" s="3" t="s">
+      <c r="G10" s="7"/>
+      <c r="H10" s="7"/>
+      <c r="I10" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="J10" s="3">
+      <c r="J10" s="7">
         <f>J8/J9</f>
         <v>120</v>
       </c>
-      <c r="M10" s="3" t="s">
+      <c r="K10" s="7"/>
+      <c r="L10" s="7"/>
+      <c r="M10" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="N10" s="3">
+      <c r="N10" s="7">
         <f>N8/N9</f>
         <v>76</v>
       </c>
-      <c r="Q10" s="3" t="s">
+      <c r="O10" s="7"/>
+      <c r="P10" s="7"/>
+      <c r="Q10" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="R10" s="15">
+      <c r="R10" s="20">
         <f>ROUND(3+(U4-R4)*(6-3)/(250-R4),2)</f>
         <v>3.2</v>
       </c>
-      <c r="T10" s="3" t="s">
+      <c r="S10" s="7"/>
+      <c r="T10" s="7" t="s">
         <v>23</v>
       </c>
       <c r="U10" s="6">
@@ -1160,22 +1229,32 @@
         <v>4.24</v>
       </c>
     </row>
-    <row r="11" spans="2:21" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:21">
       <c r="F11" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="G11" s="3">
+      <c r="G11" s="7">
         <f>ROUND(ATAN(G9/(G6*PI()))*180/PI(),3)</f>
         <v>7.1150000000000002</v>
       </c>
-      <c r="Q11" s="3" t="s">
+      <c r="H11" s="7"/>
+      <c r="I11" s="7"/>
+      <c r="J11" s="7"/>
+      <c r="K11" s="7"/>
+      <c r="L11" s="7"/>
+      <c r="M11" s="7"/>
+      <c r="N11" s="7"/>
+      <c r="O11" s="7"/>
+      <c r="P11" s="7"/>
+      <c r="Q11" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="R11" s="3">
+      <c r="R11" s="7">
         <f>ROUND(R9/J5,2)</f>
         <v>4.38</v>
       </c>
-      <c r="T11" s="3" t="s">
+      <c r="S11" s="7"/>
+      <c r="T11" s="7" t="s">
         <v>31</v>
       </c>
       <c r="U11" s="6">
@@ -1183,49 +1262,89 @@
         <v>5.72</v>
       </c>
     </row>
-    <row r="12" spans="2:21" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:21">
       <c r="F12" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="G12" s="3">
+      <c r="G12" s="7">
         <f>ROUND(ATAN(C9/COS(15*PI()/180))*180/PI(),3)</f>
         <v>5.9109999999999996</v>
       </c>
+      <c r="H12" s="7"/>
+      <c r="I12" s="7"/>
+      <c r="J12" s="7"/>
+      <c r="K12" s="7"/>
+      <c r="L12" s="7"/>
+      <c r="M12" s="7"/>
+      <c r="N12" s="7"/>
+      <c r="O12" s="7"/>
+      <c r="P12" s="7"/>
+      <c r="Q12" s="7"/>
+      <c r="R12" s="7"/>
+      <c r="S12" s="7"/>
+      <c r="T12" s="7"/>
       <c r="U12" s="6"/>
     </row>
-    <row r="13" spans="2:21" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:21">
       <c r="F13" s="5"/>
+      <c r="G13" s="7"/>
+      <c r="H13" s="7"/>
+      <c r="I13" s="7"/>
+      <c r="J13" s="7"/>
+      <c r="K13" s="7"/>
+      <c r="L13" s="7"/>
+      <c r="M13" s="7"/>
+      <c r="N13" s="7"/>
+      <c r="O13" s="7"/>
+      <c r="P13" s="7"/>
+      <c r="Q13" s="7"/>
+      <c r="R13" s="7"/>
+      <c r="S13" s="7"/>
+      <c r="T13" s="7"/>
       <c r="U13" s="6"/>
     </row>
-    <row r="14" spans="2:21" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:21">
       <c r="F14" s="16" t="s">
         <v>15</v>
       </c>
       <c r="G14" s="17"/>
+      <c r="H14" s="7"/>
+      <c r="I14" s="7"/>
+      <c r="J14" s="7"/>
+      <c r="K14" s="7"/>
+      <c r="L14" s="7"/>
+      <c r="M14" s="7"/>
+      <c r="N14" s="7"/>
+      <c r="O14" s="7"/>
+      <c r="P14" s="7"/>
+      <c r="Q14" s="7"/>
+      <c r="R14" s="7"/>
+      <c r="S14" s="7"/>
+      <c r="T14" s="7"/>
       <c r="U14" s="6"/>
     </row>
-    <row r="15" spans="2:21" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:21">
       <c r="F15" s="18" t="b">
         <f>G11&lt;G12</f>
         <v>0</v>
       </c>
       <c r="G15" s="19"/>
-      <c r="H15" s="9"/>
-      <c r="I15" s="9"/>
-      <c r="J15" s="9"/>
-      <c r="K15" s="9"/>
-      <c r="L15" s="9"/>
-      <c r="M15" s="9"/>
-      <c r="N15" s="9"/>
-      <c r="O15" s="9"/>
-      <c r="P15" s="9"/>
-      <c r="Q15" s="9"/>
-      <c r="R15" s="9"/>
-      <c r="S15" s="9"/>
-      <c r="T15" s="9"/>
-      <c r="U15" s="8"/>
-    </row>
-    <row r="18" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="H15" s="10"/>
+      <c r="I15" s="10"/>
+      <c r="J15" s="10"/>
+      <c r="K15" s="10"/>
+      <c r="L15" s="10"/>
+      <c r="M15" s="10"/>
+      <c r="N15" s="10"/>
+      <c r="O15" s="10"/>
+      <c r="P15" s="10"/>
+      <c r="Q15" s="10"/>
+      <c r="R15" s="10"/>
+      <c r="S15" s="10"/>
+      <c r="T15" s="10"/>
+      <c r="U15" s="9"/>
+    </row>
+    <row r="18" spans="1:23">
       <c r="A18" s="1"/>
       <c r="B18" s="4"/>
       <c r="C18" s="4"/>
@@ -1251,7 +1370,7 @@
         <v>43</v>
       </c>
       <c r="Q18" s="4">
-        <v>110</v>
+        <v>90</v>
       </c>
       <c r="R18" s="4"/>
       <c r="S18" s="4" t="s">
@@ -1259,29 +1378,30 @@
       </c>
       <c r="T18" s="4">
         <f>ROUND(0.5*(Q19*Q19+2*Q18*Q19+Q18*Q20)/(Q18+Q19),2)</f>
-        <v>76.63</v>
+        <v>58.91</v>
       </c>
       <c r="U18" s="4"/>
       <c r="V18" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="W18" s="12">
+      <c r="W18" s="13">
         <f>C2*(C3-K19/2)</f>
         <v>4655000</v>
       </c>
     </row>
-    <row r="19" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:23">
       <c r="A19" s="5"/>
-      <c r="B19" s="10" t="s">
+      <c r="B19" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="C19" s="10" t="s">
+      <c r="C19" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="E19" s="10" t="s">
+      <c r="D19" s="7"/>
+      <c r="E19" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="F19" s="10" t="s">
+      <c r="F19" s="11" t="s">
         <v>10</v>
       </c>
       <c r="G19" s="6"/>
@@ -1292,45 +1412,48 @@
         <f>K18*2.5</f>
         <v>70</v>
       </c>
-      <c r="M19" s="7" t="s">
+      <c r="M19" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="N19" s="8">
+      <c r="N19" s="9">
         <v>500</v>
       </c>
       <c r="P19" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="Q19" s="3">
-        <v>90</v>
-      </c>
-      <c r="S19" s="3" t="s">
+      <c r="Q19" s="7">
+        <v>70</v>
+      </c>
+      <c r="R19" s="7"/>
+      <c r="S19" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="T19" s="3">
+      <c r="T19" s="7">
         <f>Q19+Q20/2</f>
-        <v>102.5</v>
-      </c>
-      <c r="V19" s="3" t="s">
+        <v>77.5</v>
+      </c>
+      <c r="U19" s="7"/>
+      <c r="V19" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="W19" s="13">
+      <c r="W19" s="14">
         <f>ROUND(Q18*POWER(Q20,3)/12+T21*T21*Q20*Q18+Q20*POWER(Q19,3)/12+T22*T22*Q20*Q19,0)</f>
-        <v>5753464</v>
-      </c>
-    </row>
-    <row r="20" spans="1:23" x14ac:dyDescent="0.3">
+        <v>1520879</v>
+      </c>
+    </row>
+    <row r="20" spans="1:23">
       <c r="A20" s="5"/>
-      <c r="B20" s="10" t="s">
+      <c r="B20" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="C20" s="10">
+      <c r="C20" s="11">
         <v>36</v>
       </c>
-      <c r="E20" s="10" t="s">
+      <c r="D20" s="7"/>
+      <c r="E20" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="F20" s="10">
+      <c r="F20" s="11">
         <v>32</v>
       </c>
       <c r="G20" s="6"/>
@@ -1339,36 +1462,39 @@
       <c r="P20" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="Q20" s="3">
-        <v>25</v>
-      </c>
-      <c r="S20" s="3" t="s">
+      <c r="Q20" s="7">
+        <v>15</v>
+      </c>
+      <c r="R20" s="7"/>
+      <c r="S20" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="T20" s="3">
+      <c r="T20" s="7">
         <f>Q19/2</f>
-        <v>45</v>
-      </c>
-      <c r="V20" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="U20" s="7"/>
+      <c r="V20" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="W20" s="14">
+      <c r="W20" s="15">
         <f>W19/T18</f>
-        <v>75081.090956544445</v>
-      </c>
-    </row>
-    <row r="21" spans="1:23" x14ac:dyDescent="0.3">
+        <v>25816.99202172806</v>
+      </c>
+    </row>
+    <row r="21" spans="1:23">
       <c r="A21" s="5"/>
-      <c r="B21" s="10" t="s">
+      <c r="B21" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="C21" s="10">
+      <c r="C21" s="11">
         <v>33</v>
       </c>
-      <c r="E21" s="10" t="s">
+      <c r="D21" s="7"/>
+      <c r="E21" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="F21" s="10">
+      <c r="F21" s="11">
         <v>29</v>
       </c>
       <c r="G21" s="6"/>
@@ -1382,37 +1508,40 @@
       <c r="P21" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="Q21" s="3">
+      <c r="Q21" s="7">
         <f>Q20*(Q18+Q19)</f>
-        <v>5000</v>
-      </c>
-      <c r="S21" s="3" t="s">
+        <v>2400</v>
+      </c>
+      <c r="R21" s="7"/>
+      <c r="S21" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="T21" s="3">
+      <c r="T21" s="7">
         <f>T19-T18</f>
-        <v>25.870000000000005</v>
-      </c>
-      <c r="V21" s="3" t="s">
+        <v>18.590000000000003</v>
+      </c>
+      <c r="U21" s="7"/>
+      <c r="V21" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="W21" s="14">
+      <c r="W21" s="15">
         <f>W19/(Q19+Q20-T18)</f>
-        <v>149946.93771175397</v>
-      </c>
-    </row>
-    <row r="22" spans="1:23" x14ac:dyDescent="0.3">
+        <v>58293.560751245677</v>
+      </c>
+    </row>
+    <row r="22" spans="1:23">
       <c r="A22" s="5"/>
-      <c r="B22" s="10" t="s">
+      <c r="B22" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="C22" s="10">
+      <c r="C22" s="11">
         <v>29</v>
       </c>
-      <c r="E22" s="10" t="s">
+      <c r="D22" s="7"/>
+      <c r="E22" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="F22" s="10">
+      <c r="F22" s="11">
         <v>25</v>
       </c>
       <c r="G22" s="6"/>
@@ -1424,48 +1553,59 @@
         <v>2.5</v>
       </c>
       <c r="P22" s="5"/>
-      <c r="S22" s="3" t="s">
+      <c r="R22" s="7"/>
+      <c r="S22" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="T22" s="3">
+      <c r="T22" s="7">
         <f>T18-T20</f>
-        <v>31.629999999999995</v>
-      </c>
+        <v>23.909999999999997</v>
+      </c>
+      <c r="U22" s="7"/>
+      <c r="V22" s="7"/>
       <c r="W22" s="6"/>
     </row>
-    <row r="23" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:23">
       <c r="A23" s="5"/>
-      <c r="B23" s="10" t="s">
+      <c r="B23" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="C23" s="10">
+      <c r="C23" s="11">
         <v>6</v>
       </c>
-      <c r="E23" s="10" t="s">
+      <c r="D23" s="7"/>
+      <c r="E23" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="F23" s="10">
+      <c r="F23" s="11">
         <v>6</v>
       </c>
       <c r="G23" s="6"/>
       <c r="J23" s="5"/>
       <c r="K23" s="6"/>
       <c r="P23" s="5"/>
+      <c r="Q23" s="7"/>
+      <c r="R23" s="7"/>
+      <c r="S23" s="7"/>
+      <c r="T23" s="7"/>
+      <c r="U23" s="7"/>
+      <c r="V23" s="7"/>
       <c r="W23" s="6"/>
     </row>
-    <row r="24" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:23">
       <c r="A24" s="5"/>
-      <c r="B24" s="10" t="s">
+      <c r="B24" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="C24" s="10">
+      <c r="C24" s="11">
         <f>2*C23</f>
         <v>12</v>
       </c>
-      <c r="E24" s="10" t="s">
+      <c r="D24" s="7"/>
+      <c r="E24" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="F24" s="10">
+      <c r="F24" s="11">
         <f>2*F23</f>
         <v>12</v>
       </c>
@@ -1477,257 +1617,323 @@
         <v>10</v>
       </c>
       <c r="P24" s="5"/>
+      <c r="Q24" s="7"/>
+      <c r="R24" s="7"/>
+      <c r="S24" s="7"/>
+      <c r="T24" s="7"/>
+      <c r="U24" s="7"/>
+      <c r="V24" s="7"/>
       <c r="W24" s="6"/>
     </row>
-    <row r="25" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:23">
       <c r="A25" s="5"/>
+      <c r="B25" s="7"/>
+      <c r="C25" s="7"/>
+      <c r="D25" s="7"/>
+      <c r="E25" s="7"/>
+      <c r="F25" s="7"/>
       <c r="G25" s="6"/>
-      <c r="J25" s="7" t="s">
+      <c r="J25" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="K25" s="8">
+      <c r="K25" s="9">
         <f>ROUND(C2*G8/(K21*PI()*K22*K19),2)</f>
         <v>6.78</v>
       </c>
       <c r="P25" s="5"/>
-      <c r="Q25" s="3" t="s">
+      <c r="Q25" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="R25" s="3">
+      <c r="R25" s="7">
         <f>-ROUND(W18/W20,2)</f>
-        <v>-62</v>
-      </c>
-      <c r="T25" s="3" t="s">
+        <v>-180.31</v>
+      </c>
+      <c r="S25" s="7"/>
+      <c r="T25" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="U25" s="3">
-        <v>60</v>
-      </c>
+      <c r="U25" s="7">
+        <v>160</v>
+      </c>
+      <c r="V25" s="7"/>
       <c r="W25" s="6"/>
     </row>
-    <row r="26" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:23">
       <c r="A26" s="5"/>
-      <c r="B26" s="10" t="s">
+      <c r="B26" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="C26" s="10" t="s">
+      <c r="C26" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="E26" s="11" t="s">
+      <c r="D26" s="7"/>
+      <c r="E26" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="F26" s="11" t="s">
+      <c r="F26" s="12" t="s">
         <v>10</v>
       </c>
       <c r="G26" s="6"/>
       <c r="P26" s="5"/>
-      <c r="Q26" s="3" t="s">
+      <c r="Q26" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="R26" s="3">
+      <c r="R26" s="7">
         <f>ROUND(W18/W21,2)</f>
-        <v>31.04</v>
-      </c>
-      <c r="T26" s="3" t="s">
+        <v>79.849999999999994</v>
+      </c>
+      <c r="S26" s="7"/>
+      <c r="T26" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="U26" s="3">
-        <v>160</v>
-      </c>
+      <c r="U26" s="7">
+        <v>500</v>
+      </c>
+      <c r="V26" s="7"/>
       <c r="W26" s="6"/>
     </row>
-    <row r="27" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:23">
       <c r="A27" s="5"/>
-      <c r="B27" s="10" t="s">
+      <c r="B27" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="C27" s="10">
+      <c r="C27" s="11">
         <v>28</v>
       </c>
-      <c r="E27" s="11" t="s">
+      <c r="D27" s="7"/>
+      <c r="E27" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="F27" s="11">
+      <c r="F27" s="12">
         <v>24</v>
       </c>
       <c r="G27" s="6"/>
       <c r="P27" s="5"/>
-      <c r="Q27" s="3" t="s">
+      <c r="Q27" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="R27" s="3">
+      <c r="R27" s="7">
         <f>ROUND(C2/Q21,2)</f>
-        <v>3.8</v>
-      </c>
+        <v>7.92</v>
+      </c>
+      <c r="S27" s="7"/>
+      <c r="T27" s="7"/>
+      <c r="U27" s="7"/>
+      <c r="V27" s="7"/>
       <c r="W27" s="6"/>
     </row>
-    <row r="28" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:23">
       <c r="A28" s="5"/>
-      <c r="B28" s="10" t="s">
+      <c r="B28" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="C28" s="10">
+      <c r="C28" s="11">
         <v>25.5</v>
       </c>
-      <c r="E28" s="11" t="s">
+      <c r="D28" s="7"/>
+      <c r="E28" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="F28" s="11">
+      <c r="F28" s="12">
         <v>21.5</v>
       </c>
       <c r="G28" s="6"/>
       <c r="P28" s="5"/>
-      <c r="T28" s="3" t="s">
+      <c r="Q28" s="7"/>
+      <c r="R28" s="7"/>
+      <c r="S28" s="7"/>
+      <c r="T28" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="U28" s="3">
+      <c r="U28" s="7">
         <f>ABS(R25+R27)</f>
-        <v>58.2</v>
-      </c>
-      <c r="V28" s="15">
+        <v>172.39000000000001</v>
+      </c>
+      <c r="V28" s="20">
         <f>ROUND(U26/U28,2)</f>
-        <v>2.75</v>
+        <v>2.9</v>
       </c>
       <c r="W28" s="6"/>
     </row>
-    <row r="29" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:23">
       <c r="A29" s="5"/>
-      <c r="B29" s="10" t="s">
+      <c r="B29" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="C29" s="10">
+      <c r="C29" s="11">
         <v>22.5</v>
       </c>
-      <c r="E29" s="11" t="s">
+      <c r="D29" s="7"/>
+      <c r="E29" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="F29" s="11">
+      <c r="F29" s="12">
         <v>18.5</v>
       </c>
       <c r="G29" s="6"/>
-      <c r="P29" s="7"/>
-      <c r="Q29" s="9"/>
-      <c r="R29" s="9"/>
-      <c r="S29" s="9"/>
-      <c r="T29" s="9" t="s">
+      <c r="P29" s="8"/>
+      <c r="Q29" s="10"/>
+      <c r="R29" s="10"/>
+      <c r="S29" s="10"/>
+      <c r="T29" s="10" t="s">
         <v>59</v>
       </c>
-      <c r="U29" s="9">
+      <c r="U29" s="10">
         <f>R26+R27</f>
-        <v>34.839999999999996</v>
-      </c>
-      <c r="V29" s="9">
+        <v>87.77</v>
+      </c>
+      <c r="V29" s="10">
         <f>ROUND(U25/U29,2)</f>
-        <v>1.72</v>
-      </c>
-      <c r="W29" s="8"/>
-    </row>
-    <row r="30" spans="1:23" x14ac:dyDescent="0.3">
+        <v>1.82</v>
+      </c>
+      <c r="W29" s="9"/>
+    </row>
+    <row r="30" spans="1:23">
       <c r="A30" s="5"/>
-      <c r="B30" s="10" t="s">
+      <c r="B30" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="C30" s="10">
+      <c r="C30" s="11">
         <v>5</v>
       </c>
-      <c r="E30" s="11" t="s">
+      <c r="D30" s="7"/>
+      <c r="E30" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="F30" s="11">
+      <c r="F30" s="12">
         <v>5</v>
       </c>
       <c r="G30" s="6"/>
     </row>
-    <row r="31" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:23">
       <c r="A31" s="5"/>
-      <c r="B31" s="10" t="s">
+      <c r="B31" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="C31" s="10">
+      <c r="C31" s="11">
         <f>2*C30</f>
         <v>10</v>
       </c>
-      <c r="E31" s="11" t="s">
+      <c r="D31" s="7"/>
+      <c r="E31" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="F31" s="11">
+      <c r="F31" s="12">
         <f>2*F30</f>
         <v>10</v>
       </c>
       <c r="G31" s="6"/>
     </row>
-    <row r="32" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:23">
       <c r="A32" s="5"/>
+      <c r="B32" s="7"/>
+      <c r="C32" s="7"/>
+      <c r="D32" s="7"/>
+      <c r="E32" s="7"/>
+      <c r="F32" s="7"/>
       <c r="G32" s="6"/>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:7">
       <c r="A33" s="5"/>
-      <c r="B33" s="11" t="s">
+      <c r="B33" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="C33" s="11" t="s">
+      <c r="C33" s="12" t="s">
         <v>10</v>
       </c>
+      <c r="D33" s="7"/>
+      <c r="E33" s="7"/>
+      <c r="F33" s="7"/>
       <c r="G33" s="6"/>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:7">
       <c r="A34" s="5"/>
-      <c r="B34" s="11" t="s">
+      <c r="B34" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="C34" s="11">
+      <c r="C34" s="12">
         <v>20</v>
       </c>
+      <c r="D34" s="7"/>
+      <c r="E34" s="7"/>
+      <c r="F34" s="7"/>
       <c r="G34" s="6"/>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:7">
       <c r="A35" s="5"/>
-      <c r="B35" s="11" t="s">
+      <c r="B35" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="C35" s="11">
+      <c r="C35" s="12">
         <v>18</v>
       </c>
+      <c r="D35" s="7"/>
+      <c r="E35" s="7"/>
+      <c r="F35" s="7"/>
       <c r="G35" s="6"/>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:7">
       <c r="A36" s="5"/>
-      <c r="B36" s="11" t="s">
+      <c r="B36" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="C36" s="11">
+      <c r="C36" s="12">
         <v>15.5</v>
       </c>
+      <c r="D36" s="7"/>
+      <c r="E36" s="7"/>
+      <c r="F36" s="7"/>
       <c r="G36" s="6"/>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:7">
       <c r="A37" s="5"/>
-      <c r="B37" s="11" t="s">
+      <c r="B37" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="C37" s="11">
+      <c r="C37" s="12">
         <v>4</v>
       </c>
+      <c r="D37" s="7"/>
+      <c r="E37" s="7"/>
+      <c r="F37" s="7"/>
       <c r="G37" s="6"/>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B38" s="11" t="s">
+    <row r="38" spans="1:7">
+      <c r="B38" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="C38" s="11">
+      <c r="C38" s="12">
         <f>2*C37</f>
         <v>8</v>
       </c>
+      <c r="D38" s="7"/>
+      <c r="E38" s="7"/>
+      <c r="F38" s="7"/>
       <c r="G38" s="6"/>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A39" s="7"/>
-      <c r="B39" s="9"/>
-      <c r="C39" s="9"/>
-      <c r="D39" s="9"/>
-      <c r="E39" s="9"/>
-      <c r="F39" s="9"/>
-      <c r="G39" s="8"/>
+    <row r="39" spans="1:7">
+      <c r="A39" s="8"/>
+      <c r="B39" s="10"/>
+      <c r="C39" s="10"/>
+      <c r="D39" s="10"/>
+      <c r="E39" s="10"/>
+      <c r="F39" s="10"/>
+      <c r="G39" s="9"/>
+    </row>
+    <row r="40" spans="1:7">
+      <c r="B40" s="7"/>
+      <c r="C40" s="7"/>
+      <c r="D40" s="7"/>
+    </row>
+    <row r="41" spans="1:7">
+      <c r="B41" s="7"/>
+      <c r="C41" s="7"/>
+      <c r="D41" s="7"/>
+    </row>
+    <row r="42" spans="1:7">
+      <c r="B42" s="7"/>
+      <c r="C42" s="7"/>
+      <c r="D42" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -1752,52 +1958,52 @@
       <formula>$J$10</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K25">
-    <cfRule type="cellIs" dxfId="15" priority="5" operator="greaterThan">
-      <formula>$K$24</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="14" priority="6" operator="lessThanOrEqual">
-      <formula>$K$24</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="N6">
-    <cfRule type="cellIs" dxfId="13" priority="17" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="15" priority="17" operator="greaterThan">
       <formula>$N$10</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="18" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="14" priority="18" operator="lessThanOrEqual">
       <formula>$N$10</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R7">
-    <cfRule type="cellIs" dxfId="11" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="15" operator="equal">
       <formula>FALSE</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="16" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="R11">
-    <cfRule type="cellIs" dxfId="9" priority="7" operator="lessThan">
-      <formula>$R$10</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="8" operator="greaterThanOrEqual">
-      <formula>$R$10</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="U7">
-    <cfRule type="cellIs" dxfId="7" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="13" operator="equal">
       <formula>FALSE</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="14" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U11">
-    <cfRule type="cellIs" dxfId="5" priority="9" operator="lessThan">
+    <cfRule type="cellIs" dxfId="9" priority="9" operator="lessThan">
       <formula>$U$10</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="10" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="8" priority="10" operator="greaterThanOrEqual">
       <formula>$U$10</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="R11">
+    <cfRule type="cellIs" dxfId="7" priority="7" operator="lessThan">
+      <formula>$R$10</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="6" priority="8" operator="greaterThanOrEqual">
+      <formula>$R$10</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K25">
+    <cfRule type="cellIs" dxfId="5" priority="5" operator="greaterThan">
+      <formula>$K$24</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="4" priority="6" operator="lessThanOrEqual">
+      <formula>$K$24</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U28">

</xml_diff>